<commit_message>
Add SSW extraction to REMARK column for RCL rates
Implement SSW detection and extraction from column F:
- Detects "SSW" in column F ETD data
- Extracts "SSW" to REMARK column
- Removes "SSW" from dates before ETD BKK/LCH processing
- Remaining dates follow normal ETD extraction rules

Example:
- Input: "SSW / FRI (BKK PAT) / SAT (LCH)"
- Result: ETD BKK = "FRI", ETD LCH = "SAT", REMARK = "SSW"

Successfully processed 24 rows with SSW markers in current data.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/output/FINAL_RATES_FROM_ATTACHMENTS.xlsx
+++ b/docs/output/FINAL_RATES_FROM_ATTACHMENTS.xlsx
@@ -1189,7 +1189,7 @@
     <t>13 Days</t>
   </si>
   <si>
-    <t>THU (SSW &amp; LCH)</t>
+    <t>SSW</t>
   </si>
   <si>
     <t>Nanhai</t>
@@ -1939,7 +1939,7 @@
     <col min="9" max="9" width="6.998" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="5.856" bestFit="true" customWidth="true" style="0"/>
     <col min="11" max="11" width="31.707" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="18.71" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="16.425" bestFit="true" customWidth="true" style="0"/>
     <col min="13" max="13" width="12.854" bestFit="true" customWidth="true" style="0"/>
     <col min="14" max="14" width="26.993" bestFit="true" customWidth="true" style="0"/>
     <col min="15" max="15" width="19.995" bestFit="true" customWidth="true" style="0"/>
@@ -13754,9 +13754,6 @@
       <c r="G373">
         <v>50</v>
       </c>
-      <c r="L373" t="s">
-        <v>388</v>
-      </c>
       <c r="M373" t="s">
         <v>347</v>
       </c>
@@ -13769,6 +13766,9 @@
       <c r="P373" t="s">
         <v>218</v>
       </c>
+      <c r="Q373" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="374" spans="1:21">
       <c r="A374" t="s">
@@ -13792,9 +13792,6 @@
       <c r="G374">
         <v>200</v>
       </c>
-      <c r="L374" t="s">
-        <v>388</v>
-      </c>
       <c r="N374" t="s">
         <v>271</v>
       </c>
@@ -13804,6 +13801,9 @@
       <c r="P374" t="s">
         <v>218</v>
       </c>
+      <c r="Q374" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="375" spans="1:21">
       <c r="A375" t="s">
@@ -13827,9 +13827,6 @@
       <c r="G375">
         <v>50</v>
       </c>
-      <c r="L375" t="s">
-        <v>388</v>
-      </c>
       <c r="M375" t="s">
         <v>364</v>
       </c>
@@ -13842,6 +13839,9 @@
       <c r="P375" t="s">
         <v>218</v>
       </c>
+      <c r="Q375" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="376" spans="1:21">
       <c r="A376" t="s">
@@ -13865,9 +13865,6 @@
       <c r="G376">
         <v>200</v>
       </c>
-      <c r="L376" t="s">
-        <v>388</v>
-      </c>
       <c r="N376" t="s">
         <v>271</v>
       </c>
@@ -13877,6 +13874,9 @@
       <c r="P376" t="s">
         <v>218</v>
       </c>
+      <c r="Q376" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="377" spans="1:21">
       <c r="A377" t="s">
@@ -13900,9 +13900,6 @@
       <c r="G377">
         <v>450</v>
       </c>
-      <c r="L377" t="s">
-        <v>388</v>
-      </c>
       <c r="M377" t="s">
         <v>390</v>
       </c>
@@ -13915,6 +13912,9 @@
       <c r="P377" t="s">
         <v>218</v>
       </c>
+      <c r="Q377" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="378" spans="1:21">
       <c r="A378" t="s">
@@ -13938,9 +13938,6 @@
       <c r="G378">
         <v>600</v>
       </c>
-      <c r="L378" t="s">
-        <v>388</v>
-      </c>
       <c r="N378" t="s">
         <v>391</v>
       </c>
@@ -13950,6 +13947,9 @@
       <c r="P378" t="s">
         <v>218</v>
       </c>
+      <c r="Q378" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="379" spans="1:21">
       <c r="A379" t="s">
@@ -13973,9 +13973,6 @@
       <c r="G379">
         <v>300</v>
       </c>
-      <c r="L379" t="s">
-        <v>388</v>
-      </c>
       <c r="M379" t="s">
         <v>390</v>
       </c>
@@ -13988,6 +13985,9 @@
       <c r="P379" t="s">
         <v>218</v>
       </c>
+      <c r="Q379" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="380" spans="1:21">
       <c r="A380" t="s">
@@ -14011,9 +14011,6 @@
       <c r="G380">
         <v>450</v>
       </c>
-      <c r="L380" t="s">
-        <v>388</v>
-      </c>
       <c r="N380" t="s">
         <v>391</v>
       </c>
@@ -14023,6 +14020,9 @@
       <c r="P380" t="s">
         <v>218</v>
       </c>
+      <c r="Q380" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="381" spans="1:21">
       <c r="A381" t="s">
@@ -14046,9 +14046,6 @@
       <c r="G381">
         <v>300</v>
       </c>
-      <c r="L381" t="s">
-        <v>388</v>
-      </c>
       <c r="M381" t="s">
         <v>390</v>
       </c>
@@ -14061,6 +14058,9 @@
       <c r="P381" t="s">
         <v>218</v>
       </c>
+      <c r="Q381" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="382" spans="1:21">
       <c r="A382" t="s">
@@ -14084,9 +14084,6 @@
       <c r="G382">
         <v>450</v>
       </c>
-      <c r="L382" t="s">
-        <v>388</v>
-      </c>
       <c r="N382" t="s">
         <v>391</v>
       </c>
@@ -14096,6 +14093,9 @@
       <c r="P382" t="s">
         <v>218</v>
       </c>
+      <c r="Q382" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="383" spans="1:21">
       <c r="A383" t="s">
@@ -14119,9 +14119,6 @@
       <c r="G383">
         <v>300</v>
       </c>
-      <c r="L383" t="s">
-        <v>388</v>
-      </c>
       <c r="M383" t="s">
         <v>390</v>
       </c>
@@ -14134,6 +14131,9 @@
       <c r="P383" t="s">
         <v>218</v>
       </c>
+      <c r="Q383" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="384" spans="1:21">
       <c r="A384" t="s">
@@ -14157,9 +14157,6 @@
       <c r="G384">
         <v>450</v>
       </c>
-      <c r="L384" t="s">
-        <v>388</v>
-      </c>
       <c r="N384" t="s">
         <v>391</v>
       </c>
@@ -14169,6 +14166,9 @@
       <c r="P384" t="s">
         <v>218</v>
       </c>
+      <c r="Q384" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="385" spans="1:21">
       <c r="A385" t="s">
@@ -14192,9 +14192,6 @@
       <c r="G385">
         <v>300</v>
       </c>
-      <c r="L385" t="s">
-        <v>388</v>
-      </c>
       <c r="M385" t="s">
         <v>390</v>
       </c>
@@ -14207,6 +14204,9 @@
       <c r="P385" t="s">
         <v>218</v>
       </c>
+      <c r="Q385" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="386" spans="1:21">
       <c r="A386" t="s">
@@ -14230,9 +14230,6 @@
       <c r="G386">
         <v>450</v>
       </c>
-      <c r="L386" t="s">
-        <v>388</v>
-      </c>
       <c r="N386" t="s">
         <v>391</v>
       </c>
@@ -14242,6 +14239,9 @@
       <c r="P386" t="s">
         <v>218</v>
       </c>
+      <c r="Q386" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="387" spans="1:21">
       <c r="A387" t="s">
@@ -14265,9 +14265,6 @@
       <c r="G387">
         <v>300</v>
       </c>
-      <c r="L387" t="s">
-        <v>388</v>
-      </c>
       <c r="M387" t="s">
         <v>390</v>
       </c>
@@ -14280,6 +14277,9 @@
       <c r="P387" t="s">
         <v>218</v>
       </c>
+      <c r="Q387" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="388" spans="1:21">
       <c r="A388" t="s">
@@ -14303,9 +14303,6 @@
       <c r="G388">
         <v>450</v>
       </c>
-      <c r="L388" t="s">
-        <v>388</v>
-      </c>
       <c r="N388" t="s">
         <v>391</v>
       </c>
@@ -14315,6 +14312,9 @@
       <c r="P388" t="s">
         <v>218</v>
       </c>
+      <c r="Q388" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="389" spans="1:21">
       <c r="A389" t="s">
@@ -14338,9 +14338,6 @@
       <c r="G389">
         <v>300</v>
       </c>
-      <c r="L389" t="s">
-        <v>388</v>
-      </c>
       <c r="M389" t="s">
         <v>390</v>
       </c>
@@ -14353,6 +14350,9 @@
       <c r="P389" t="s">
         <v>218</v>
       </c>
+      <c r="Q389" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="390" spans="1:21">
       <c r="A390" t="s">
@@ -14376,9 +14376,6 @@
       <c r="G390">
         <v>450</v>
       </c>
-      <c r="L390" t="s">
-        <v>388</v>
-      </c>
       <c r="N390" t="s">
         <v>391</v>
       </c>
@@ -14388,6 +14385,9 @@
       <c r="P390" t="s">
         <v>218</v>
       </c>
+      <c r="Q390" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="391" spans="1:21">
       <c r="A391" t="s">
@@ -14411,9 +14411,6 @@
       <c r="G391">
         <v>300</v>
       </c>
-      <c r="L391" t="s">
-        <v>388</v>
-      </c>
       <c r="M391" t="s">
         <v>390</v>
       </c>
@@ -14426,6 +14423,9 @@
       <c r="P391" t="s">
         <v>218</v>
       </c>
+      <c r="Q391" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="392" spans="1:21">
       <c r="A392" t="s">
@@ -14449,9 +14449,6 @@
       <c r="G392">
         <v>450</v>
       </c>
-      <c r="L392" t="s">
-        <v>388</v>
-      </c>
       <c r="N392" t="s">
         <v>391</v>
       </c>
@@ -14461,6 +14458,9 @@
       <c r="P392" t="s">
         <v>218</v>
       </c>
+      <c r="Q392" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="393" spans="1:21">
       <c r="A393" t="s">
@@ -14484,9 +14484,6 @@
       <c r="G393">
         <v>300</v>
       </c>
-      <c r="L393" t="s">
-        <v>388</v>
-      </c>
       <c r="M393" t="s">
         <v>390</v>
       </c>
@@ -14499,6 +14496,9 @@
       <c r="P393" t="s">
         <v>218</v>
       </c>
+      <c r="Q393" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="394" spans="1:21">
       <c r="A394" t="s">
@@ -14522,9 +14522,6 @@
       <c r="G394">
         <v>450</v>
       </c>
-      <c r="L394" t="s">
-        <v>388</v>
-      </c>
       <c r="N394" t="s">
         <v>391</v>
       </c>
@@ -14534,6 +14531,9 @@
       <c r="P394" t="s">
         <v>218</v>
       </c>
+      <c r="Q394" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="395" spans="1:21">
       <c r="A395" t="s">
@@ -14557,9 +14557,6 @@
       <c r="G395">
         <v>300</v>
       </c>
-      <c r="L395" t="s">
-        <v>388</v>
-      </c>
       <c r="M395" t="s">
         <v>390</v>
       </c>
@@ -14572,6 +14569,9 @@
       <c r="P395" t="s">
         <v>218</v>
       </c>
+      <c r="Q395" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="396" spans="1:21">
       <c r="A396" t="s">
@@ -14595,9 +14595,6 @@
       <c r="G396">
         <v>450</v>
       </c>
-      <c r="L396" t="s">
-        <v>388</v>
-      </c>
       <c r="N396" t="s">
         <v>391</v>
       </c>
@@ -14606,6 +14603,9 @@
       </c>
       <c r="P396" t="s">
         <v>218</v>
+      </c>
+      <c r="Q396" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="397" spans="1:21">

</xml_diff>

<commit_message>
Fix SSW extraction to preserve ETD dates with SSW indicator
Corrected SSW logic to properly handle dates containing SSW:
- Dates like "THU (SSW & LCH)" now extract to ETD LCH as "THU"
- Dates like "FRI (SSW & BKK PAT)" now extract to ETD BKK as "FRI"
- SSW is still extracted to REMARK column
- Only standalone "SSW" (without LCH/BKK) is skipped for ETD processing

Previous behavior incorrectly removed all SSW-containing dates.
Now dates with SSW + LCH/BKK indicators are properly extracted.

Example results:
- "THU (SSW & LCH)" → ETD LCH: "THU", REMARK: "SSW"
- "SSW / FRI (BKK PAT)" → ETD BKK: "FRI", REMARK: "SSW"

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/output/FINAL_RATES_FROM_ATTACHMENTS.xlsx
+++ b/docs/output/FINAL_RATES_FROM_ATTACHMENTS.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="512">
   <si>
     <t>CARRIER</t>
   </si>
@@ -1207,16 +1207,10 @@
     <t>Dongguan</t>
   </si>
   <si>
-    <t>SUN (LCH)</t>
-  </si>
-  <si>
     <t>5 Days</t>
   </si>
   <si>
     <t>7 DEM + 7 DET</t>
-  </si>
-  <si>
-    <t>WED (LCH)</t>
   </si>
   <si>
     <t>8 DEM + 6 DET</t>
@@ -13754,6 +13748,9 @@
       <c r="G373">
         <v>50</v>
       </c>
+      <c r="L373" t="s">
+        <v>36</v>
+      </c>
       <c r="M373" t="s">
         <v>347</v>
       </c>
@@ -13792,6 +13789,9 @@
       <c r="G374">
         <v>200</v>
       </c>
+      <c r="L374" t="s">
+        <v>36</v>
+      </c>
       <c r="N374" t="s">
         <v>271</v>
       </c>
@@ -13827,6 +13827,9 @@
       <c r="G375">
         <v>50</v>
       </c>
+      <c r="L375" t="s">
+        <v>36</v>
+      </c>
       <c r="M375" t="s">
         <v>364</v>
       </c>
@@ -13865,6 +13868,9 @@
       <c r="G376">
         <v>200</v>
       </c>
+      <c r="L376" t="s">
+        <v>36</v>
+      </c>
       <c r="N376" t="s">
         <v>271</v>
       </c>
@@ -13900,6 +13906,9 @@
       <c r="G377">
         <v>450</v>
       </c>
+      <c r="L377" t="s">
+        <v>36</v>
+      </c>
       <c r="M377" t="s">
         <v>390</v>
       </c>
@@ -13938,6 +13947,9 @@
       <c r="G378">
         <v>600</v>
       </c>
+      <c r="L378" t="s">
+        <v>36</v>
+      </c>
       <c r="N378" t="s">
         <v>391</v>
       </c>
@@ -13973,6 +13985,9 @@
       <c r="G379">
         <v>300</v>
       </c>
+      <c r="L379" t="s">
+        <v>36</v>
+      </c>
       <c r="M379" t="s">
         <v>390</v>
       </c>
@@ -14011,6 +14026,9 @@
       <c r="G380">
         <v>450</v>
       </c>
+      <c r="L380" t="s">
+        <v>36</v>
+      </c>
       <c r="N380" t="s">
         <v>391</v>
       </c>
@@ -14046,6 +14064,9 @@
       <c r="G381">
         <v>300</v>
       </c>
+      <c r="L381" t="s">
+        <v>36</v>
+      </c>
       <c r="M381" t="s">
         <v>390</v>
       </c>
@@ -14084,6 +14105,9 @@
       <c r="G382">
         <v>450</v>
       </c>
+      <c r="L382" t="s">
+        <v>36</v>
+      </c>
       <c r="N382" t="s">
         <v>391</v>
       </c>
@@ -14119,6 +14143,9 @@
       <c r="G383">
         <v>300</v>
       </c>
+      <c r="L383" t="s">
+        <v>36</v>
+      </c>
       <c r="M383" t="s">
         <v>390</v>
       </c>
@@ -14157,6 +14184,9 @@
       <c r="G384">
         <v>450</v>
       </c>
+      <c r="L384" t="s">
+        <v>36</v>
+      </c>
       <c r="N384" t="s">
         <v>391</v>
       </c>
@@ -14192,6 +14222,9 @@
       <c r="G385">
         <v>300</v>
       </c>
+      <c r="L385" t="s">
+        <v>36</v>
+      </c>
       <c r="M385" t="s">
         <v>390</v>
       </c>
@@ -14230,6 +14263,9 @@
       <c r="G386">
         <v>450</v>
       </c>
+      <c r="L386" t="s">
+        <v>36</v>
+      </c>
       <c r="N386" t="s">
         <v>391</v>
       </c>
@@ -14265,6 +14301,9 @@
       <c r="G387">
         <v>300</v>
       </c>
+      <c r="L387" t="s">
+        <v>36</v>
+      </c>
       <c r="M387" t="s">
         <v>390</v>
       </c>
@@ -14303,6 +14342,9 @@
       <c r="G388">
         <v>450</v>
       </c>
+      <c r="L388" t="s">
+        <v>36</v>
+      </c>
       <c r="N388" t="s">
         <v>391</v>
       </c>
@@ -14338,6 +14380,9 @@
       <c r="G389">
         <v>300</v>
       </c>
+      <c r="L389" t="s">
+        <v>36</v>
+      </c>
       <c r="M389" t="s">
         <v>390</v>
       </c>
@@ -14376,6 +14421,9 @@
       <c r="G390">
         <v>450</v>
       </c>
+      <c r="L390" t="s">
+        <v>36</v>
+      </c>
       <c r="N390" t="s">
         <v>391</v>
       </c>
@@ -14411,6 +14459,9 @@
       <c r="G391">
         <v>300</v>
       </c>
+      <c r="L391" t="s">
+        <v>36</v>
+      </c>
       <c r="M391" t="s">
         <v>390</v>
       </c>
@@ -14449,6 +14500,9 @@
       <c r="G392">
         <v>450</v>
       </c>
+      <c r="L392" t="s">
+        <v>36</v>
+      </c>
       <c r="N392" t="s">
         <v>391</v>
       </c>
@@ -14484,6 +14538,9 @@
       <c r="G393">
         <v>300</v>
       </c>
+      <c r="L393" t="s">
+        <v>36</v>
+      </c>
       <c r="M393" t="s">
         <v>390</v>
       </c>
@@ -14522,6 +14579,9 @@
       <c r="G394">
         <v>450</v>
       </c>
+      <c r="L394" t="s">
+        <v>36</v>
+      </c>
       <c r="N394" t="s">
         <v>391</v>
       </c>
@@ -14557,6 +14617,9 @@
       <c r="G395">
         <v>300</v>
       </c>
+      <c r="L395" t="s">
+        <v>36</v>
+      </c>
       <c r="M395" t="s">
         <v>390</v>
       </c>
@@ -14595,6 +14658,9 @@
       <c r="G396">
         <v>450</v>
       </c>
+      <c r="L396" t="s">
+        <v>36</v>
+      </c>
       <c r="N396" t="s">
         <v>391</v>
       </c>
@@ -14631,16 +14697,16 @@
         <v>120</v>
       </c>
       <c r="L397" t="s">
+        <v>338</v>
+      </c>
+      <c r="M397" t="s">
         <v>394</v>
-      </c>
-      <c r="M397" t="s">
-        <v>395</v>
       </c>
       <c r="N397" t="s">
         <v>271</v>
       </c>
       <c r="O397" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="P397" t="s">
         <v>218</v>
@@ -14669,16 +14735,16 @@
         <v>270</v>
       </c>
       <c r="L398" t="s">
+        <v>338</v>
+      </c>
+      <c r="M398" t="s">
         <v>394</v>
-      </c>
-      <c r="M398" t="s">
-        <v>395</v>
       </c>
       <c r="N398" t="s">
         <v>271</v>
       </c>
       <c r="O398" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="P398" t="s">
         <v>218</v>
@@ -14707,7 +14773,7 @@
         <v>400</v>
       </c>
       <c r="L399" t="s">
-        <v>397</v>
+        <v>23</v>
       </c>
       <c r="M399" t="s">
         <v>364</v>
@@ -14716,7 +14782,7 @@
         <v>271</v>
       </c>
       <c r="O399" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="P399" t="s">
         <v>218</v>
@@ -14745,7 +14811,7 @@
         <v>550</v>
       </c>
       <c r="L400" t="s">
-        <v>397</v>
+        <v>23</v>
       </c>
       <c r="M400" t="s">
         <v>364</v>
@@ -14754,7 +14820,7 @@
         <v>271</v>
       </c>
       <c r="O400" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="P400" t="s">
         <v>218</v>
@@ -14783,7 +14849,7 @@
         <v>400</v>
       </c>
       <c r="L401" t="s">
-        <v>397</v>
+        <v>23</v>
       </c>
       <c r="M401" t="s">
         <v>364</v>
@@ -14792,7 +14858,7 @@
         <v>271</v>
       </c>
       <c r="O401" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="P401" t="s">
         <v>218</v>
@@ -14821,7 +14887,7 @@
         <v>550</v>
       </c>
       <c r="L402" t="s">
-        <v>397</v>
+        <v>23</v>
       </c>
       <c r="M402" t="s">
         <v>364</v>
@@ -14830,7 +14896,7 @@
         <v>271</v>
       </c>
       <c r="O402" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="P402" t="s">
         <v>218</v>
@@ -14844,7 +14910,7 @@
         <v>273</v>
       </c>
       <c r="C403" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D403" t="s">
         <v>22</v>
@@ -14885,7 +14951,7 @@
         <v>235</v>
       </c>
       <c r="C404" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D404" t="s">
         <v>22</v>
@@ -14923,7 +14989,7 @@
         <v>268</v>
       </c>
       <c r="C405" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D405" t="s">
         <v>22</v>
@@ -14961,7 +15027,7 @@
         <v>273</v>
       </c>
       <c r="C406" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D406" t="s">
         <v>22</v>
@@ -14982,7 +15048,7 @@
         <v>34</v>
       </c>
       <c r="M406" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="N406" t="s">
         <v>276</v>
@@ -15002,7 +15068,7 @@
         <v>235</v>
       </c>
       <c r="C407" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D407" t="s">
         <v>22</v>
@@ -15020,7 +15086,7 @@
         <v>277</v>
       </c>
       <c r="M407" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="N407" t="s">
         <v>276</v>
@@ -15040,7 +15106,7 @@
         <v>268</v>
       </c>
       <c r="C408" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D408" t="s">
         <v>22</v>
@@ -15058,7 +15124,7 @@
         <v>277</v>
       </c>
       <c r="M408" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="N408" t="s">
         <v>276</v>
@@ -15078,7 +15144,7 @@
         <v>273</v>
       </c>
       <c r="C409" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D409" t="s">
         <v>22</v>
@@ -15099,7 +15165,7 @@
         <v>361</v>
       </c>
       <c r="M409" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="N409" t="s">
         <v>367</v>
@@ -15140,7 +15206,7 @@
         <v>361</v>
       </c>
       <c r="M410" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="N410" t="s">
         <v>367</v>
@@ -15181,7 +15247,7 @@
         <v>361</v>
       </c>
       <c r="M411" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="N411" t="s">
         <v>367</v>
@@ -15222,7 +15288,7 @@
         <v>361</v>
       </c>
       <c r="M412" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="N412" t="s">
         <v>367</v>
@@ -15263,7 +15329,7 @@
         <v>361</v>
       </c>
       <c r="M413" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="N413" t="s">
         <v>367</v>
@@ -15283,7 +15349,7 @@
         <v>273</v>
       </c>
       <c r="C414" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D414" t="s">
         <v>22</v>
@@ -15304,7 +15370,7 @@
         <v>361</v>
       </c>
       <c r="M414" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="N414" t="s">
         <v>367</v>
@@ -15345,7 +15411,7 @@
         <v>361</v>
       </c>
       <c r="M415" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="N415" t="s">
         <v>367</v>
@@ -15365,7 +15431,7 @@
         <v>273</v>
       </c>
       <c r="C416" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D416" t="s">
         <v>22</v>
@@ -15386,7 +15452,7 @@
         <v>361</v>
       </c>
       <c r="M416" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="N416" t="s">
         <v>367</v>
@@ -15406,7 +15472,7 @@
         <v>273</v>
       </c>
       <c r="C417" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D417" t="s">
         <v>22</v>
@@ -15427,7 +15493,7 @@
         <v>361</v>
       </c>
       <c r="M417" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="N417" t="s">
         <v>367</v>
@@ -15447,7 +15513,7 @@
         <v>273</v>
       </c>
       <c r="C418" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D418" t="s">
         <v>22</v>
@@ -15468,7 +15534,7 @@
         <v>361</v>
       </c>
       <c r="M418" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="N418" t="s">
         <v>367</v>
@@ -15482,13 +15548,13 @@
     </row>
     <row r="419" spans="1:21">
       <c r="A419" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B419" t="s">
         <v>217</v>
       </c>
       <c r="C419" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D419" t="s">
         <v>22</v>
@@ -15508,13 +15574,13 @@
     </row>
     <row r="420" spans="1:21">
       <c r="A420" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B420" t="s">
         <v>217</v>
       </c>
       <c r="C420" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D420" t="s">
         <v>22</v>
@@ -15534,13 +15600,13 @@
     </row>
     <row r="421" spans="1:21">
       <c r="A421" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B421" t="s">
         <v>217</v>
       </c>
       <c r="C421" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D421" t="s">
         <v>22</v>
@@ -15560,13 +15626,13 @@
     </row>
     <row r="422" spans="1:21">
       <c r="A422" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B422" t="s">
         <v>217</v>
       </c>
       <c r="C422" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D422" t="s">
         <v>22</v>
@@ -15586,13 +15652,13 @@
     </row>
     <row r="423" spans="1:21">
       <c r="A423" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B423" t="s">
         <v>217</v>
       </c>
       <c r="C423" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D423" t="s">
         <v>22</v>
@@ -15612,13 +15678,13 @@
     </row>
     <row r="424" spans="1:21">
       <c r="A424" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B424" t="s">
         <v>217</v>
       </c>
       <c r="C424" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D424" t="s">
         <v>22</v>
@@ -15638,13 +15704,13 @@
     </row>
     <row r="425" spans="1:21">
       <c r="A425" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B425" t="s">
         <v>217</v>
       </c>
       <c r="C425" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D425" t="s">
         <v>22</v>
@@ -15664,13 +15730,13 @@
     </row>
     <row r="426" spans="1:21">
       <c r="A426" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B426" t="s">
         <v>217</v>
       </c>
       <c r="C426" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D426" t="s">
         <v>22</v>
@@ -15690,13 +15756,13 @@
     </row>
     <row r="427" spans="1:21">
       <c r="A427" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B427" t="s">
         <v>217</v>
       </c>
       <c r="C427" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D427" t="s">
         <v>22</v>
@@ -15716,13 +15782,13 @@
     </row>
     <row r="428" spans="1:21">
       <c r="A428" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B428" t="s">
         <v>217</v>
       </c>
       <c r="C428" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D428" t="s">
         <v>22</v>
@@ -15742,13 +15808,13 @@
     </row>
     <row r="429" spans="1:21">
       <c r="A429" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B429" t="s">
         <v>217</v>
       </c>
       <c r="C429" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D429" t="s">
         <v>22</v>
@@ -15768,13 +15834,13 @@
     </row>
     <row r="430" spans="1:21">
       <c r="A430" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B430" t="s">
         <v>217</v>
       </c>
       <c r="C430" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D430" t="s">
         <v>22</v>
@@ -15794,13 +15860,13 @@
     </row>
     <row r="431" spans="1:21">
       <c r="A431" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B431" t="s">
         <v>217</v>
       </c>
       <c r="C431" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D431" t="s">
         <v>22</v>
@@ -15820,13 +15886,13 @@
     </row>
     <row r="432" spans="1:21">
       <c r="A432" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B432" t="s">
         <v>217</v>
       </c>
       <c r="C432" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D432" t="s">
         <v>22</v>
@@ -15846,13 +15912,13 @@
     </row>
     <row r="433" spans="1:21">
       <c r="A433" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B433" t="s">
         <v>217</v>
       </c>
       <c r="C433" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D433" t="s">
         <v>22</v>
@@ -15872,13 +15938,13 @@
     </row>
     <row r="434" spans="1:21">
       <c r="A434" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B434" t="s">
         <v>217</v>
       </c>
       <c r="C434" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D434" t="s">
         <v>22</v>
@@ -15898,13 +15964,13 @@
     </row>
     <row r="435" spans="1:21">
       <c r="A435" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B435" t="s">
         <v>217</v>
       </c>
       <c r="C435" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D435" t="s">
         <v>22</v>
@@ -15924,13 +15990,13 @@
     </row>
     <row r="436" spans="1:21">
       <c r="A436" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B436" t="s">
         <v>217</v>
       </c>
       <c r="C436" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D436" t="s">
         <v>22</v>
@@ -15950,13 +16016,13 @@
     </row>
     <row r="437" spans="1:21">
       <c r="A437" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B437" t="s">
         <v>217</v>
       </c>
       <c r="C437" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D437" t="s">
         <v>22</v>
@@ -15976,13 +16042,13 @@
     </row>
     <row r="438" spans="1:21">
       <c r="A438" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B438" t="s">
         <v>217</v>
       </c>
       <c r="C438" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D438" t="s">
         <v>22</v>
@@ -16002,13 +16068,13 @@
     </row>
     <row r="439" spans="1:21">
       <c r="A439" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B439" t="s">
         <v>217</v>
       </c>
       <c r="C439" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D439" t="s">
         <v>22</v>
@@ -16028,13 +16094,13 @@
     </row>
     <row r="440" spans="1:21">
       <c r="A440" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B440" t="s">
         <v>217</v>
       </c>
       <c r="C440" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D440" t="s">
         <v>22</v>
@@ -16054,13 +16120,13 @@
     </row>
     <row r="441" spans="1:21">
       <c r="A441" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B441" t="s">
         <v>217</v>
       </c>
       <c r="C441" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D441" t="s">
         <v>22</v>
@@ -16080,13 +16146,13 @@
     </row>
     <row r="442" spans="1:21">
       <c r="A442" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B442" t="s">
         <v>217</v>
       </c>
       <c r="C442" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D442" t="s">
         <v>22</v>
@@ -16106,13 +16172,13 @@
     </row>
     <row r="443" spans="1:21">
       <c r="A443" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B443" t="s">
         <v>217</v>
       </c>
       <c r="C443" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D443" t="s">
         <v>22</v>
@@ -16132,13 +16198,13 @@
     </row>
     <row r="444" spans="1:21">
       <c r="A444" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B444" t="s">
         <v>217</v>
       </c>
       <c r="C444" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D444" t="s">
         <v>22</v>
@@ -16158,13 +16224,13 @@
     </row>
     <row r="445" spans="1:21">
       <c r="A445" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B445" t="s">
         <v>217</v>
       </c>
       <c r="C445" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D445" t="s">
         <v>22</v>
@@ -16184,13 +16250,13 @@
     </row>
     <row r="446" spans="1:21">
       <c r="A446" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B446" t="s">
         <v>217</v>
       </c>
       <c r="C446" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D446" t="s">
         <v>22</v>
@@ -16210,13 +16276,13 @@
     </row>
     <row r="447" spans="1:21">
       <c r="A447" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B447" t="s">
         <v>217</v>
       </c>
       <c r="C447" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D447" t="s">
         <v>22</v>
@@ -16236,13 +16302,13 @@
     </row>
     <row r="448" spans="1:21">
       <c r="A448" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B448" t="s">
         <v>217</v>
       </c>
       <c r="C448" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D448" t="s">
         <v>22</v>
@@ -16262,13 +16328,13 @@
     </row>
     <row r="449" spans="1:21">
       <c r="A449" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B449" t="s">
         <v>217</v>
       </c>
       <c r="C449" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D449" t="s">
         <v>22</v>
@@ -16288,13 +16354,13 @@
     </row>
     <row r="450" spans="1:21">
       <c r="A450" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B450" t="s">
         <v>217</v>
       </c>
       <c r="C450" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D450" t="s">
         <v>22</v>
@@ -16314,13 +16380,13 @@
     </row>
     <row r="451" spans="1:21">
       <c r="A451" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B451" t="s">
         <v>217</v>
       </c>
       <c r="C451" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D451" t="s">
         <v>22</v>
@@ -16340,13 +16406,13 @@
     </row>
     <row r="452" spans="1:21">
       <c r="A452" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B452" t="s">
         <v>217</v>
       </c>
       <c r="C452" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="D452" t="s">
         <v>22</v>
@@ -16366,13 +16432,13 @@
     </row>
     <row r="453" spans="1:21">
       <c r="A453" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B453" t="s">
         <v>217</v>
       </c>
       <c r="C453" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D453" t="s">
         <v>22</v>
@@ -16392,13 +16458,13 @@
     </row>
     <row r="454" spans="1:21">
       <c r="A454" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B454" t="s">
         <v>217</v>
       </c>
       <c r="C454" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D454" t="s">
         <v>22</v>
@@ -16418,13 +16484,13 @@
     </row>
     <row r="455" spans="1:21">
       <c r="A455" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B455" t="s">
         <v>217</v>
       </c>
       <c r="C455" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D455" t="s">
         <v>22</v>
@@ -16444,13 +16510,13 @@
     </row>
     <row r="456" spans="1:21">
       <c r="A456" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B456" t="s">
         <v>217</v>
       </c>
       <c r="C456" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D456" t="s">
         <v>22</v>
@@ -16470,10 +16536,10 @@
     </row>
     <row r="457" spans="1:21">
       <c r="A457" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C457" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D457" t="s">
         <v>22</v>
@@ -16490,10 +16556,10 @@
     </row>
     <row r="458" spans="1:21">
       <c r="A458" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C458" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D458" t="s">
         <v>22</v>
@@ -16510,10 +16576,10 @@
     </row>
     <row r="459" spans="1:21">
       <c r="A459" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C459" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D459" t="s">
         <v>22</v>
@@ -16530,10 +16596,10 @@
     </row>
     <row r="460" spans="1:21">
       <c r="A460" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C460" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D460" t="s">
         <v>22</v>
@@ -16550,10 +16616,10 @@
     </row>
     <row r="461" spans="1:21">
       <c r="A461" t="s">
+        <v>445</v>
+      </c>
+      <c r="C461" t="s">
         <v>447</v>
-      </c>
-      <c r="C461" t="s">
-        <v>449</v>
       </c>
       <c r="D461" t="s">
         <v>22</v>
@@ -16570,13 +16636,13 @@
     </row>
     <row r="462" spans="1:21">
       <c r="A462" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B462" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C462" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D462" t="s">
         <v>22</v>
@@ -16593,10 +16659,10 @@
     </row>
     <row r="463" spans="1:21">
       <c r="A463" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C463" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D463" t="s">
         <v>22</v>
@@ -16613,13 +16679,13 @@
     </row>
     <row r="464" spans="1:21">
       <c r="A464" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B464" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C464" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D464" t="s">
         <v>22</v>
@@ -16636,10 +16702,10 @@
     </row>
     <row r="465" spans="1:21">
       <c r="A465" t="s">
+        <v>445</v>
+      </c>
+      <c r="C465" t="s">
         <v>447</v>
-      </c>
-      <c r="C465" t="s">
-        <v>449</v>
       </c>
       <c r="D465" t="s">
         <v>22</v>
@@ -16656,13 +16722,13 @@
     </row>
     <row r="466" spans="1:21">
       <c r="A466" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B466" t="s">
         <v>86</v>
       </c>
       <c r="C466" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D466" t="s">
         <v>22</v>
@@ -16679,13 +16745,13 @@
     </row>
     <row r="467" spans="1:21">
       <c r="A467" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B467" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C467" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D467" t="s">
         <v>22</v>
@@ -16702,13 +16768,13 @@
     </row>
     <row r="468" spans="1:21">
       <c r="A468" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B468" t="s">
         <v>93</v>
       </c>
       <c r="C468" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D468" t="s">
         <v>22</v>
@@ -16725,13 +16791,13 @@
     </row>
     <row r="469" spans="1:21">
       <c r="A469" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B469" t="s">
         <v>378</v>
       </c>
       <c r="C469" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D469" t="s">
         <v>22</v>
@@ -16748,10 +16814,10 @@
     </row>
     <row r="470" spans="1:21">
       <c r="A470" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C470" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D470" t="s">
         <v>22</v>
@@ -16771,10 +16837,10 @@
     </row>
     <row r="471" spans="1:21">
       <c r="A471" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C471" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D471" t="s">
         <v>22</v>
@@ -16791,13 +16857,13 @@
     </row>
     <row r="472" spans="1:21">
       <c r="A472" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B472" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C472" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D472" t="s">
         <v>22</v>
@@ -16812,18 +16878,18 @@
         <v>2</v>
       </c>
       <c r="M472" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="473" spans="1:21">
       <c r="A473" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B473" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C473" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D473" t="s">
         <v>22</v>
@@ -16838,15 +16904,15 @@
         <v>8</v>
       </c>
       <c r="M473" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="474" spans="1:21">
       <c r="A474" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C474" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D474" t="s">
         <v>22</v>
@@ -16863,10 +16929,10 @@
     </row>
     <row r="475" spans="1:21">
       <c r="A475" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C475" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D475" t="s">
         <v>22</v>
@@ -16881,15 +16947,15 @@
         <v>11</v>
       </c>
       <c r="M475" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="476" spans="1:21">
       <c r="A476" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C476" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D476" t="s">
         <v>22</v>
@@ -16909,10 +16975,10 @@
     </row>
     <row r="477" spans="1:21">
       <c r="A477" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C477" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D477" t="s">
         <v>22</v>
@@ -16932,13 +16998,13 @@
     </row>
     <row r="478" spans="1:21">
       <c r="A478" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B478" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C478" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D478" t="s">
         <v>22</v>
@@ -16958,10 +17024,10 @@
     </row>
     <row r="479" spans="1:21">
       <c r="A479" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C479" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D479" t="s">
         <v>22</v>
@@ -16978,10 +17044,10 @@
     </row>
     <row r="480" spans="1:21">
       <c r="A480" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C480" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D480" t="s">
         <v>22</v>
@@ -17001,10 +17067,10 @@
     </row>
     <row r="481" spans="1:21">
       <c r="A481" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C481" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D481" t="s">
         <v>22</v>
@@ -17019,15 +17085,15 @@
         <v>4</v>
       </c>
       <c r="M481" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="482" spans="1:21">
       <c r="A482" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C482" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D482" t="s">
         <v>22</v>
@@ -17047,10 +17113,10 @@
     </row>
     <row r="483" spans="1:21">
       <c r="A483" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C483" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D483" t="s">
         <v>22</v>
@@ -17070,10 +17136,10 @@
     </row>
     <row r="484" spans="1:21">
       <c r="A484" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C484" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D484" t="s">
         <v>22</v>
@@ -17093,13 +17159,13 @@
     </row>
     <row r="485" spans="1:21">
       <c r="A485" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B485" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C485" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D485" t="s">
         <v>22</v>
@@ -17116,13 +17182,13 @@
     </row>
     <row r="486" spans="1:21">
       <c r="A486" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B486" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C486" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D486" t="s">
         <v>22</v>
@@ -17139,13 +17205,13 @@
     </row>
     <row r="487" spans="1:21">
       <c r="A487" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B487" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C487" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D487" t="s">
         <v>22</v>
@@ -17162,13 +17228,13 @@
     </row>
     <row r="488" spans="1:21">
       <c r="A488" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B488" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C488" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D488" t="s">
         <v>22</v>
@@ -17185,13 +17251,13 @@
     </row>
     <row r="489" spans="1:21">
       <c r="A489" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B489" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C489" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D489" t="s">
         <v>22</v>
@@ -17206,18 +17272,18 @@
         <v>200</v>
       </c>
       <c r="K489" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="490" spans="1:21">
       <c r="A490" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B490" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C490" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D490" t="s">
         <v>22</v>
@@ -17234,13 +17300,13 @@
     </row>
     <row r="491" spans="1:21">
       <c r="A491" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B491" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C491" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D491" t="s">
         <v>22</v>
@@ -17257,13 +17323,13 @@
     </row>
     <row r="492" spans="1:21">
       <c r="A492" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B492" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C492" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D492" t="s">
         <v>22</v>
@@ -17280,13 +17346,13 @@
     </row>
     <row r="493" spans="1:21">
       <c r="A493" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B493" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C493" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D493" t="s">
         <v>22</v>
@@ -17301,18 +17367,18 @@
         <v>1</v>
       </c>
       <c r="K493" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="494" spans="1:21">
       <c r="A494" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B494" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C494" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D494" t="s">
         <v>22</v>
@@ -17327,18 +17393,18 @@
         <v>400</v>
       </c>
       <c r="K494" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="495" spans="1:21">
       <c r="A495" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B495" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C495" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D495" t="s">
         <v>22</v>
@@ -17355,13 +17421,13 @@
     </row>
     <row r="496" spans="1:21">
       <c r="A496" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B496" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C496" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D496" t="s">
         <v>22</v>
@@ -17378,13 +17444,13 @@
     </row>
     <row r="497" spans="1:21">
       <c r="A497" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B497" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C497" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D497" t="s">
         <v>22</v>
@@ -17401,13 +17467,13 @@
     </row>
     <row r="498" spans="1:21">
       <c r="A498" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B498" t="s">
         <v>346</v>
       </c>
       <c r="C498" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D498" t="s">
         <v>22</v>
@@ -17424,13 +17490,13 @@
     </row>
     <row r="499" spans="1:21">
       <c r="A499" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B499" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C499" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D499" t="s">
         <v>22</v>
@@ -17447,13 +17513,13 @@
     </row>
     <row r="500" spans="1:21">
       <c r="A500" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B500" t="s">
         <v>340</v>
       </c>
       <c r="C500" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D500" t="s">
         <v>22</v>
@@ -17470,10 +17536,10 @@
     </row>
     <row r="501" spans="1:21">
       <c r="A501" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C501" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D501" t="s">
         <v>22</v>
@@ -17490,10 +17556,10 @@
     </row>
     <row r="502" spans="1:21">
       <c r="A502" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C502" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D502" t="s">
         <v>22</v>
@@ -17510,13 +17576,13 @@
     </row>
     <row r="503" spans="1:21">
       <c r="A503" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B503" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C503" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D503" t="s">
         <v>22</v>
@@ -17533,10 +17599,10 @@
     </row>
     <row r="504" spans="1:21">
       <c r="A504" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C504" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D504" t="s">
         <v>22</v>
@@ -17553,13 +17619,13 @@
     </row>
     <row r="505" spans="1:21">
       <c r="A505" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B505" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C505" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D505" t="s">
         <v>22</v>
@@ -17576,10 +17642,10 @@
     </row>
     <row r="506" spans="1:21">
       <c r="A506" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C506" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D506" t="s">
         <v>22</v>
@@ -17596,10 +17662,10 @@
     </row>
     <row r="507" spans="1:21">
       <c r="A507" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C507" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D507" t="s">
         <v>22</v>
@@ -17619,10 +17685,10 @@
     </row>
     <row r="508" spans="1:21">
       <c r="A508" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C508" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D508" t="s">
         <v>22</v>
@@ -17639,10 +17705,10 @@
     </row>
     <row r="509" spans="1:21">
       <c r="A509" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C509" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D509" t="s">
         <v>22</v>
@@ -17659,10 +17725,10 @@
     </row>
     <row r="510" spans="1:21">
       <c r="A510" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C510" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D510" t="s">
         <v>22</v>
@@ -17679,10 +17745,10 @@
     </row>
     <row r="511" spans="1:21">
       <c r="A511" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C511" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D511" t="s">
         <v>22</v>
@@ -17699,10 +17765,10 @@
     </row>
     <row r="512" spans="1:21">
       <c r="A512" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C512" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D512" t="s">
         <v>22</v>
@@ -17719,10 +17785,10 @@
     </row>
     <row r="513" spans="1:21">
       <c r="A513" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C513" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D513" t="s">
         <v>22</v>
@@ -17739,10 +17805,10 @@
     </row>
     <row r="514" spans="1:21">
       <c r="A514" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C514" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D514" t="s">
         <v>22</v>
@@ -17759,10 +17825,10 @@
     </row>
     <row r="515" spans="1:21">
       <c r="A515" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C515" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D515" t="s">
         <v>22</v>
@@ -17779,10 +17845,10 @@
     </row>
     <row r="516" spans="1:21">
       <c r="A516" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C516" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D516" t="s">
         <v>22</v>
@@ -17799,10 +17865,10 @@
     </row>
     <row r="517" spans="1:21">
       <c r="A517" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C517" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D517" t="s">
         <v>22</v>
@@ -17819,13 +17885,13 @@
     </row>
     <row r="518" spans="1:21">
       <c r="A518" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B518" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C518" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D518" t="s">
         <v>22</v>
@@ -17842,13 +17908,13 @@
     </row>
     <row r="519" spans="1:21">
       <c r="A519" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B519" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C519" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D519" t="s">
         <v>22</v>
@@ -17865,13 +17931,13 @@
     </row>
     <row r="520" spans="1:21">
       <c r="A520" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B520" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C520" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D520" t="s">
         <v>22</v>
@@ -17888,10 +17954,10 @@
     </row>
     <row r="521" spans="1:21">
       <c r="A521" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C521" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D521" t="s">
         <v>22</v>
@@ -17908,13 +17974,13 @@
     </row>
     <row r="522" spans="1:21">
       <c r="A522" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B522" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C522" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D522" t="s">
         <v>22</v>
@@ -17931,10 +17997,10 @@
     </row>
     <row r="523" spans="1:21">
       <c r="A523" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C523" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D523" t="s">
         <v>22</v>
@@ -17951,13 +18017,13 @@
     </row>
     <row r="524" spans="1:21">
       <c r="A524" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B524" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C524" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D524" t="s">
         <v>22</v>
@@ -17974,10 +18040,10 @@
     </row>
     <row r="525" spans="1:21">
       <c r="A525" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C525" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="D525" t="s">
         <v>22</v>
@@ -17994,13 +18060,13 @@
     </row>
     <row r="526" spans="1:21">
       <c r="A526" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B526" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C526" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D526" t="s">
         <v>22</v>
@@ -18017,10 +18083,10 @@
     </row>
     <row r="527" spans="1:21">
       <c r="A527" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C527" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="D527" t="s">
         <v>22</v>
@@ -18037,13 +18103,13 @@
     </row>
     <row r="528" spans="1:21">
       <c r="A528" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B528" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C528" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D528" t="s">
         <v>22</v>
@@ -18060,10 +18126,10 @@
     </row>
     <row r="529" spans="1:21">
       <c r="A529" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C529" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D529" t="s">
         <v>22</v>
@@ -18080,13 +18146,13 @@
     </row>
     <row r="530" spans="1:21">
       <c r="A530" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B530" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C530" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D530" t="s">
         <v>22</v>
@@ -18103,10 +18169,10 @@
     </row>
     <row r="531" spans="1:21">
       <c r="A531" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C531" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D531" t="s">
         <v>22</v>
@@ -18123,13 +18189,13 @@
     </row>
     <row r="532" spans="1:21">
       <c r="A532" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B532" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C532" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D532" t="s">
         <v>22</v>
@@ -18146,10 +18212,10 @@
     </row>
     <row r="533" spans="1:21">
       <c r="A533" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C533" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D533" t="s">
         <v>22</v>
@@ -18166,10 +18232,10 @@
     </row>
     <row r="534" spans="1:21">
       <c r="A534" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C534" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D534" t="s">
         <v>22</v>
@@ -18189,10 +18255,10 @@
     </row>
     <row r="535" spans="1:21">
       <c r="A535" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C535" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="D535" t="s">
         <v>22</v>
@@ -18209,7 +18275,7 @@
     </row>
     <row r="536" spans="1:21">
       <c r="A536" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C536" t="s">
         <v>106</v>
@@ -18229,10 +18295,10 @@
     </row>
     <row r="537" spans="1:21">
       <c r="A537" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C537" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="D537" t="s">
         <v>22</v>
@@ -18249,10 +18315,10 @@
     </row>
     <row r="538" spans="1:21">
       <c r="A538" t="s">
+        <v>485</v>
+      </c>
+      <c r="C538" t="s">
         <v>487</v>
-      </c>
-      <c r="C538" t="s">
-        <v>489</v>
       </c>
       <c r="D538" t="s">
         <v>22</v>
@@ -18269,10 +18335,10 @@
     </row>
     <row r="539" spans="1:21">
       <c r="A539" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C539" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D539" t="s">
         <v>22</v>
@@ -18289,10 +18355,10 @@
     </row>
     <row r="540" spans="1:21">
       <c r="A540" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C540" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D540" t="s">
         <v>22</v>
@@ -18309,13 +18375,13 @@
     </row>
     <row r="541" spans="1:21">
       <c r="A541" t="s">
+        <v>490</v>
+      </c>
+      <c r="B541" t="s">
+        <v>491</v>
+      </c>
+      <c r="C541" t="s">
         <v>492</v>
-      </c>
-      <c r="B541" t="s">
-        <v>493</v>
-      </c>
-      <c r="C541" t="s">
-        <v>494</v>
       </c>
       <c r="D541" t="s">
         <v>22</v>
@@ -18332,13 +18398,13 @@
     </row>
     <row r="542" spans="1:21">
       <c r="A542" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B542" t="s">
         <v>217</v>
       </c>
       <c r="C542" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="D542" t="s">
         <v>22</v>
@@ -18358,13 +18424,13 @@
     </row>
     <row r="543" spans="1:21">
       <c r="A543" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B543" t="s">
         <v>217</v>
       </c>
       <c r="C543" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="D543" t="s">
         <v>22</v>
@@ -18384,13 +18450,13 @@
     </row>
     <row r="544" spans="1:21">
       <c r="A544" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B544" t="s">
         <v>217</v>
       </c>
       <c r="C544" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D544" t="s">
         <v>22</v>
@@ -18410,13 +18476,13 @@
     </row>
     <row r="545" spans="1:21">
       <c r="A545" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B545" t="s">
         <v>217</v>
       </c>
       <c r="C545" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D545" t="s">
         <v>22</v>
@@ -18436,13 +18502,13 @@
     </row>
     <row r="546" spans="1:21">
       <c r="A546" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B546" t="s">
         <v>217</v>
       </c>
       <c r="C546" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D546" t="s">
         <v>22</v>
@@ -18462,13 +18528,13 @@
     </row>
     <row r="547" spans="1:21">
       <c r="A547" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B547" t="s">
         <v>217</v>
       </c>
       <c r="C547" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D547" t="s">
         <v>22</v>
@@ -18488,13 +18554,13 @@
     </row>
     <row r="548" spans="1:21">
       <c r="A548" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B548" t="s">
         <v>217</v>
       </c>
       <c r="C548" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D548" t="s">
         <v>22</v>
@@ -18514,13 +18580,13 @@
     </row>
     <row r="549" spans="1:21">
       <c r="A549" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B549" t="s">
         <v>217</v>
       </c>
       <c r="C549" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D549" t="s">
         <v>22</v>
@@ -18540,13 +18606,13 @@
     </row>
     <row r="550" spans="1:21">
       <c r="A550" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B550" t="s">
         <v>217</v>
       </c>
       <c r="C550" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D550" t="s">
         <v>22</v>
@@ -18566,13 +18632,13 @@
     </row>
     <row r="551" spans="1:21">
       <c r="A551" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B551" t="s">
         <v>217</v>
       </c>
       <c r="C551" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="D551" t="s">
         <v>22</v>
@@ -18592,13 +18658,13 @@
     </row>
     <row r="552" spans="1:21">
       <c r="A552" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B552" t="s">
         <v>217</v>
       </c>
       <c r="C552" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D552" t="s">
         <v>22</v>
@@ -18618,13 +18684,13 @@
     </row>
     <row r="553" spans="1:21">
       <c r="A553" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B553" t="s">
         <v>217</v>
       </c>
       <c r="C553" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D553" t="s">
         <v>22</v>
@@ -18644,13 +18710,13 @@
     </row>
     <row r="554" spans="1:21">
       <c r="A554" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B554" t="s">
         <v>217</v>
       </c>
       <c r="C554" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D554" t="s">
         <v>22</v>
@@ -18670,13 +18736,13 @@
     </row>
     <row r="555" spans="1:21">
       <c r="A555" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B555" t="s">
         <v>217</v>
       </c>
       <c r="C555" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D555" t="s">
         <v>22</v>
@@ -18696,13 +18762,13 @@
     </row>
     <row r="556" spans="1:21">
       <c r="A556" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B556" t="s">
         <v>217</v>
       </c>
       <c r="C556" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D556" t="s">
         <v>22</v>
@@ -18722,13 +18788,13 @@
     </row>
     <row r="557" spans="1:21">
       <c r="A557" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B557" t="s">
         <v>217</v>
       </c>
       <c r="C557" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D557" t="s">
         <v>22</v>
@@ -18748,13 +18814,13 @@
     </row>
     <row r="558" spans="1:21">
       <c r="A558" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B558" t="s">
         <v>217</v>
       </c>
       <c r="C558" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D558" t="s">
         <v>22</v>
@@ -18774,13 +18840,13 @@
     </row>
     <row r="559" spans="1:21">
       <c r="A559" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B559" t="s">
         <v>217</v>
       </c>
       <c r="C559" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D559" t="s">
         <v>22</v>
@@ -18800,13 +18866,13 @@
     </row>
     <row r="560" spans="1:21">
       <c r="A560" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B560" t="s">
         <v>217</v>
       </c>
       <c r="C560" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="D560" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Format VALIDITY dates to readable format for RCL rates
Add formatValidity() function to convert date ranges to readable format:
- Takes the end date from date range (e.g., "01/11-15/11" → "15/11")
- Converts to "DD Mon YYYY" format (e.g., "15 Nov 2025")
- Defaults to year 2025 if not specified

Conversion examples:
- "01/11-15/11" → "15 Nov 2025"
- "01/11-30/11/2025" → "30 Nov 2025"

This makes VALIDITY dates much more readable and user-friendly
in the final output spreadsheet.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/output/FINAL_RATES_FROM_ATTACHMENTS.xlsx
+++ b/docs/output/FINAL_RATES_FROM_ATTACHMENTS.xlsx
@@ -829,7 +829,7 @@
     <t>14 DAYS COMBINED</t>
   </si>
   <si>
-    <t>01/11-15/11</t>
+    <t>15 Nov 2025</t>
   </si>
   <si>
     <t>Subject to local charge at both ends / Included CIC/PCS at POD</t>
@@ -1048,7 +1048,7 @@
     <t>3 Days</t>
   </si>
   <si>
-    <t>01/11-30/11/2025</t>
+    <t>30 Nov 2025</t>
   </si>
   <si>
     <t>Penang</t>
@@ -1996,7 +1996,7 @@
     <col min="13" max="13" width="12.854" bestFit="true" customWidth="true" style="0"/>
     <col min="14" max="14" width="26.993" bestFit="true" customWidth="true" style="0"/>
     <col min="15" max="15" width="19.995" bestFit="true" customWidth="true" style="0"/>
-    <col min="16" max="16" width="19.995" bestFit="true" customWidth="true" style="0"/>
+    <col min="16" max="16" width="13.997" bestFit="true" customWidth="true" style="0"/>
     <col min="17" max="17" width="93.12" bestFit="true" customWidth="true" style="0"/>
     <col min="18" max="18" width="8.141" bestFit="true" customWidth="true" style="0"/>
     <col min="19" max="19" width="10.569" bestFit="true" customWidth="true" style="0"/>

</xml_diff>

<commit_message>
Fix SITC column shift and add WANHAI ASIA remark extraction
- Fix SITC parser column shift issue in Table 5/6 where VTX service codes
  were incorrectly placed in the 20' rate column instead of REMARK
- Add Pattern 1b handling for 4-column rows (POL|POD|20'|40') without
  service route column
- Remove incorrect "repeated POD" logic that caused column misalignment
- Add WANHAI ASIA remark extraction from Azure JSON content with
  destination-to-remark mapping for Japan, Taiwan, Philippines, etc.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/output/FINAL_RATES_FROM_ATTACHMENTS.xlsx
+++ b/docs/output/FINAL_RATES_FROM_ATTACHMENTS.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="373">
   <si>
     <t>CARRIER</t>
   </si>
@@ -787,18 +787,27 @@
     <t>9-10 Days</t>
   </si>
   <si>
-    <t>Direct Days</t>
+    <t>09-Oct Days</t>
   </si>
   <si>
     <t>SHEKOU</t>
   </si>
   <si>
+    <t>5,12,4,5 Days</t>
+  </si>
+  <si>
     <t>VTX3,VTX4,VTX6</t>
   </si>
   <si>
     <t>NANSHA</t>
   </si>
   <si>
+    <t>11, 6 Days</t>
+  </si>
+  <si>
+    <t>7 days (det)</t>
+  </si>
+  <si>
     <t>VTX4, VTX5</t>
   </si>
   <si>
@@ -922,18 +931,30 @@
     <t>Kuching/Sarawak (Malay)</t>
   </si>
   <si>
+    <t>20-25 Days</t>
+  </si>
+  <si>
+    <t>7/5 days (dem+detention)</t>
+  </si>
+  <si>
     <t>Bintulu</t>
   </si>
   <si>
     <t>Jakarta (NPCT1 Terminal)</t>
   </si>
   <si>
+    <t>7 days combine dem/det</t>
+  </si>
+  <si>
     <t>LKB/NYS/Sahathai</t>
   </si>
   <si>
     <t>Cikarang (CKD)</t>
   </si>
   <si>
+    <t>T/S JKT by truck</t>
+  </si>
+  <si>
     <t>Batam/Indo (CY/CY)</t>
   </si>
   <si>
@@ -952,9 +973,15 @@
     <t>Surabaya</t>
   </si>
   <si>
+    <t>29 Days</t>
+  </si>
+  <si>
     <t>BUSAN</t>
   </si>
   <si>
+    <t>10 dem/ 5 det</t>
+  </si>
+  <si>
     <t>VTX1, VTX5</t>
   </si>
   <si>
@@ -964,6 +991,9 @@
     <t>OSAKA/KOBE</t>
   </si>
   <si>
+    <t>7 dem/ 5 det</t>
+  </si>
+  <si>
     <t>KAWASAKI</t>
   </si>
   <si>
@@ -973,6 +1003,9 @@
     <t>NGO/TOKYO/YOKO</t>
   </si>
   <si>
+    <t>12,13,14</t>
+  </si>
+  <si>
     <t>VTX3 ,VTX6</t>
   </si>
   <si>
@@ -985,6 +1018,12 @@
     <t>Tokyo/Yoko/Nagoya</t>
   </si>
   <si>
+    <t>11,12,13</t>
+  </si>
+  <si>
+    <t>7dem/ 5 det</t>
+  </si>
+  <si>
     <t>SAKAISENBOKU</t>
   </si>
   <si>
@@ -1036,30 +1075,18 @@
     <t>Chittagong (Chattogram)</t>
   </si>
   <si>
-    <t>1,150</t>
-  </si>
-  <si>
     <t>DHAKA</t>
   </si>
   <si>
-    <t>1,550</t>
-  </si>
-  <si>
     <t>Yangon /Myamar</t>
   </si>
   <si>
-    <t>1,530</t>
-  </si>
-  <si>
     <t>Chennai / India</t>
   </si>
   <si>
     <t>TPT/SHT/LKB</t>
   </si>
   <si>
-    <t>1,250</t>
-  </si>
-  <si>
     <t>Visakhapatnam / India</t>
   </si>
   <si>
@@ -1069,9 +1096,6 @@
     <t>Include LSS</t>
   </si>
   <si>
-    <t>7 dem/ 5 det</t>
-  </si>
-  <si>
     <t>Please recheck case by case(Reefer)</t>
   </si>
   <si>
@@ -1120,13 +1144,7 @@
     <t>Haldia</t>
   </si>
   <si>
-    <t>1,650</t>
-  </si>
-  <si>
     <t>Kolkata (Calcutta)</t>
-  </si>
-  <si>
-    <t>1,850</t>
   </si>
 </sst>
 </file>
@@ -8190,7 +8208,7 @@
         <v>253</v>
       </c>
       <c r="N165" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O165" t="s">
         <v>251</v>
@@ -8225,10 +8243,10 @@
         <v>70</v>
       </c>
       <c r="M166" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="N166" t="s">
-        <v>251</v>
+        <v>26</v>
       </c>
       <c r="O166" t="s">
         <v>251</v>
@@ -8237,7 +8255,7 @@
         <v>27</v>
       </c>
       <c r="Q166" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="167" spans="1:21">
@@ -8263,19 +8281,19 @@
         <v>120</v>
       </c>
       <c r="M167" t="s">
-        <v>25</v>
+        <v>255</v>
       </c>
       <c r="N167" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O167" t="s">
-        <v>25</v>
+        <v>251</v>
       </c>
       <c r="P167" t="s">
         <v>27</v>
       </c>
       <c r="Q167" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="168" spans="1:21">
@@ -8286,7 +8304,7 @@
         <v>221</v>
       </c>
       <c r="C168" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D168" t="s">
         <v>23</v>
@@ -8301,19 +8319,19 @@
         <v>80</v>
       </c>
       <c r="M168" t="s">
-        <v>25</v>
+        <v>258</v>
       </c>
       <c r="N168" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O168" t="s">
-        <v>25</v>
+        <v>259</v>
       </c>
       <c r="P168" t="s">
         <v>27</v>
       </c>
       <c r="Q168" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="169" spans="1:21">
@@ -8324,7 +8342,7 @@
         <v>225</v>
       </c>
       <c r="C169" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D169" t="s">
         <v>23</v>
@@ -8339,19 +8357,19 @@
         <v>130</v>
       </c>
       <c r="M169" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="N169" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O169" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="P169" t="s">
         <v>27</v>
       </c>
       <c r="Q169" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="170" spans="1:21">
@@ -8377,19 +8395,19 @@
         <v>70</v>
       </c>
       <c r="M170" t="s">
-        <v>253</v>
+        <v>52</v>
       </c>
       <c r="N170" t="s">
-        <v>258</v>
+        <v>26</v>
       </c>
       <c r="O170" t="s">
-        <v>251</v>
+        <v>261</v>
       </c>
       <c r="P170" t="s">
         <v>27</v>
       </c>
       <c r="Q170" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="171" spans="1:21">
@@ -8415,19 +8433,19 @@
         <v>120</v>
       </c>
       <c r="M171" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="N171" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O171" t="s">
-        <v>25</v>
+        <v>261</v>
       </c>
       <c r="P171" t="s">
         <v>27</v>
       </c>
       <c r="Q171" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="172" spans="1:21">
@@ -8438,7 +8456,7 @@
         <v>221</v>
       </c>
       <c r="C172" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="D172" t="s">
         <v>23</v>
@@ -8453,19 +8471,19 @@
         <v>100</v>
       </c>
       <c r="M172" t="s">
-        <v>25</v>
+        <v>178</v>
       </c>
       <c r="N172" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O172" t="s">
-        <v>25</v>
+        <v>251</v>
       </c>
       <c r="P172" t="s">
         <v>27</v>
       </c>
       <c r="Q172" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="173" spans="1:21">
@@ -8476,7 +8494,7 @@
         <v>225</v>
       </c>
       <c r="C173" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="D173" t="s">
         <v>23</v>
@@ -8491,19 +8509,19 @@
         <v>150</v>
       </c>
       <c r="M173" t="s">
-        <v>25</v>
+        <v>178</v>
       </c>
       <c r="N173" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O173" t="s">
-        <v>25</v>
+        <v>251</v>
       </c>
       <c r="P173" t="s">
         <v>27</v>
       </c>
       <c r="Q173" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="174" spans="1:21">
@@ -8514,7 +8532,7 @@
         <v>221</v>
       </c>
       <c r="C174" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="D174" t="s">
         <v>23</v>
@@ -8529,19 +8547,19 @@
         <v>70</v>
       </c>
       <c r="M174" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="N174" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O174" t="s">
-        <v>25</v>
+        <v>259</v>
       </c>
       <c r="P174" t="s">
         <v>27</v>
       </c>
       <c r="Q174" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="175" spans="1:21">
@@ -8552,7 +8570,7 @@
         <v>225</v>
       </c>
       <c r="C175" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="D175" t="s">
         <v>23</v>
@@ -8567,19 +8585,19 @@
         <v>120</v>
       </c>
       <c r="M175" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="N175" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O175" t="s">
-        <v>25</v>
+        <v>259</v>
       </c>
       <c r="P175" t="s">
         <v>27</v>
       </c>
       <c r="Q175" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="176" spans="1:21">
@@ -8590,7 +8608,7 @@
         <v>221</v>
       </c>
       <c r="C176" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="D176" t="s">
         <v>23</v>
@@ -8605,19 +8623,19 @@
         <v>170</v>
       </c>
       <c r="M176" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="N176" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O176" t="s">
-        <v>25</v>
+        <v>251</v>
       </c>
       <c r="P176" t="s">
         <v>27</v>
       </c>
       <c r="Q176" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="177" spans="1:21">
@@ -8628,7 +8646,7 @@
         <v>225</v>
       </c>
       <c r="C177" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="D177" t="s">
         <v>23</v>
@@ -8643,19 +8661,19 @@
         <v>220</v>
       </c>
       <c r="M177" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="N177" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O177" t="s">
-        <v>25</v>
+        <v>251</v>
       </c>
       <c r="P177" t="s">
         <v>27</v>
       </c>
       <c r="Q177" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="178" spans="1:21">
@@ -8666,7 +8684,7 @@
         <v>221</v>
       </c>
       <c r="C178" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="D178" t="s">
         <v>23</v>
@@ -8684,7 +8702,7 @@
         <v>56</v>
       </c>
       <c r="N178" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="O178" t="s">
         <v>251</v>
@@ -8704,7 +8722,7 @@
         <v>225</v>
       </c>
       <c r="C179" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="D179" t="s">
         <v>23</v>
@@ -8722,7 +8740,7 @@
         <v>56</v>
       </c>
       <c r="N179" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="O179" t="s">
         <v>251</v>
@@ -8739,10 +8757,10 @@
         <v>220</v>
       </c>
       <c r="B180" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C180" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="D180" t="s">
         <v>23</v>
@@ -8777,10 +8795,10 @@
         <v>220</v>
       </c>
       <c r="B181" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C181" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="D181" t="s">
         <v>23</v>
@@ -8788,6 +8806,12 @@
       <c r="E181">
         <v>750</v>
       </c>
+      <c r="F181">
+        <v>430</v>
+      </c>
+      <c r="G181">
+        <v>430</v>
+      </c>
       <c r="M181" t="s">
         <v>199</v>
       </c>
@@ -8812,7 +8836,7 @@
         <v>221</v>
       </c>
       <c r="C182" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="D182" t="s">
         <v>23</v>
@@ -8830,7 +8854,7 @@
         <v>56</v>
       </c>
       <c r="N182" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="O182" t="s">
         <v>251</v>
@@ -8839,7 +8863,7 @@
         <v>27</v>
       </c>
       <c r="Q182" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="183" spans="1:21">
@@ -8850,7 +8874,7 @@
         <v>225</v>
       </c>
       <c r="C183" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="D183" t="s">
         <v>23</v>
@@ -8868,7 +8892,7 @@
         <v>56</v>
       </c>
       <c r="N183" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="O183" t="s">
         <v>251</v>
@@ -8877,7 +8901,7 @@
         <v>27</v>
       </c>
       <c r="Q183" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="184" spans="1:21">
@@ -8888,7 +8912,7 @@
         <v>221</v>
       </c>
       <c r="C184" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="D184" t="s">
         <v>23</v>
@@ -8906,7 +8930,7 @@
         <v>56</v>
       </c>
       <c r="N184" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="O184" t="s">
         <v>251</v>
@@ -8915,7 +8939,7 @@
         <v>27</v>
       </c>
       <c r="Q184" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="185" spans="1:21">
@@ -8926,7 +8950,7 @@
         <v>225</v>
       </c>
       <c r="C185" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="D185" t="s">
         <v>23</v>
@@ -8941,19 +8965,19 @@
         <v>1000</v>
       </c>
       <c r="M185" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="N185" t="s">
-        <v>25</v>
+        <v>275</v>
       </c>
       <c r="O185" t="s">
-        <v>25</v>
+        <v>251</v>
       </c>
       <c r="P185" t="s">
         <v>27</v>
       </c>
       <c r="Q185" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="186" spans="1:21">
@@ -8964,7 +8988,7 @@
         <v>221</v>
       </c>
       <c r="C186" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="D186" t="s">
         <v>23</v>
@@ -8985,7 +9009,7 @@
         <v>241</v>
       </c>
       <c r="O186" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="P186" t="s">
         <v>27</v>
@@ -9002,7 +9026,7 @@
         <v>225</v>
       </c>
       <c r="C187" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="D187" t="s">
         <v>23</v>
@@ -9017,13 +9041,13 @@
         <v>200</v>
       </c>
       <c r="M187" t="s">
-        <v>25</v>
+        <v>178</v>
       </c>
       <c r="N187" t="s">
-        <v>25</v>
+        <v>241</v>
       </c>
       <c r="O187" t="s">
-        <v>25</v>
+        <v>278</v>
       </c>
       <c r="P187" t="s">
         <v>27</v>
@@ -9040,7 +9064,7 @@
         <v>221</v>
       </c>
       <c r="C188" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="D188" t="s">
         <v>23</v>
@@ -9055,13 +9079,13 @@
         <v>150</v>
       </c>
       <c r="M188" t="s">
-        <v>25</v>
+        <v>178</v>
       </c>
       <c r="N188" t="s">
-        <v>25</v>
+        <v>241</v>
       </c>
       <c r="O188" t="s">
-        <v>25</v>
+        <v>259</v>
       </c>
       <c r="P188" t="s">
         <v>27</v>
@@ -9078,7 +9102,7 @@
         <v>225</v>
       </c>
       <c r="C189" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="D189" t="s">
         <v>23</v>
@@ -9093,13 +9117,13 @@
         <v>200</v>
       </c>
       <c r="M189" t="s">
-        <v>25</v>
+        <v>178</v>
       </c>
       <c r="N189" t="s">
-        <v>25</v>
+        <v>241</v>
       </c>
       <c r="O189" t="s">
-        <v>25</v>
+        <v>259</v>
       </c>
       <c r="P189" t="s">
         <v>27</v>
@@ -9116,7 +9140,7 @@
         <v>221</v>
       </c>
       <c r="C190" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="D190" t="s">
         <v>23</v>
@@ -9134,7 +9158,7 @@
         <v>56</v>
       </c>
       <c r="N190" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="O190" t="s">
         <v>251</v>
@@ -9154,7 +9178,7 @@
         <v>225</v>
       </c>
       <c r="C191" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="D191" t="s">
         <v>23</v>
@@ -9169,13 +9193,13 @@
         <v>220</v>
       </c>
       <c r="M191" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="N191" t="s">
-        <v>25</v>
+        <v>281</v>
       </c>
       <c r="O191" t="s">
-        <v>25</v>
+        <v>251</v>
       </c>
       <c r="P191" t="s">
         <v>27</v>
@@ -9192,7 +9216,7 @@
         <v>221</v>
       </c>
       <c r="C192" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="D192" t="s">
         <v>23</v>
@@ -9207,7 +9231,7 @@
         <v>750</v>
       </c>
       <c r="M192" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="N192" t="s">
         <v>26</v>
@@ -9219,7 +9243,7 @@
         <v>27</v>
       </c>
       <c r="Q192" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="193" spans="1:21">
@@ -9227,10 +9251,10 @@
         <v>220</v>
       </c>
       <c r="B193" t="s">
+        <v>285</v>
+      </c>
+      <c r="C193" t="s">
         <v>282</v>
-      </c>
-      <c r="C193" t="s">
-        <v>279</v>
       </c>
       <c r="D193" t="s">
         <v>23</v>
@@ -9245,7 +9269,7 @@
         <v>880</v>
       </c>
       <c r="M193" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="N193" t="s">
         <v>26</v>
@@ -9257,7 +9281,7 @@
         <v>27</v>
       </c>
       <c r="Q193" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="194" spans="1:21">
@@ -9268,7 +9292,7 @@
         <v>221</v>
       </c>
       <c r="C194" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="D194" t="s">
         <v>23</v>
@@ -9283,13 +9307,13 @@
         <v>1500</v>
       </c>
       <c r="M194" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="N194" t="s">
-        <v>25</v>
+        <v>287</v>
       </c>
       <c r="O194" t="s">
-        <v>25</v>
+        <v>251</v>
       </c>
       <c r="P194" t="s">
         <v>27</v>
@@ -9306,7 +9330,7 @@
         <v>225</v>
       </c>
       <c r="C195" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="D195" t="s">
         <v>23</v>
@@ -9324,7 +9348,7 @@
         <v>77</v>
       </c>
       <c r="N195" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="O195" t="s">
         <v>251</v>
@@ -9344,7 +9368,7 @@
         <v>221</v>
       </c>
       <c r="C196" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="D196" t="s">
         <v>23</v>
@@ -9359,13 +9383,13 @@
         <v>1300</v>
       </c>
       <c r="M196" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="N196" t="s">
-        <v>25</v>
+        <v>287</v>
       </c>
       <c r="O196" t="s">
-        <v>25</v>
+        <v>251</v>
       </c>
       <c r="P196" t="s">
         <v>27</v>
@@ -9382,7 +9406,7 @@
         <v>225</v>
       </c>
       <c r="C197" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="D197" t="s">
         <v>23</v>
@@ -9400,7 +9424,7 @@
         <v>77</v>
       </c>
       <c r="N197" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="O197" t="s">
         <v>251</v>
@@ -9420,7 +9444,7 @@
         <v>221</v>
       </c>
       <c r="C198" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="D198" t="s">
         <v>23</v>
@@ -9435,19 +9459,19 @@
         <v>750</v>
       </c>
       <c r="M198" t="s">
-        <v>25</v>
+        <v>283</v>
       </c>
       <c r="N198" t="s">
-        <v>25</v>
+        <v>150</v>
       </c>
       <c r="O198" t="s">
-        <v>25</v>
+        <v>251</v>
       </c>
       <c r="P198" t="s">
         <v>27</v>
       </c>
       <c r="Q198" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="199" spans="1:21">
@@ -9455,10 +9479,10 @@
         <v>220</v>
       </c>
       <c r="B199" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="C199" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="D199" t="s">
         <v>23</v>
@@ -9473,19 +9497,19 @@
         <v>880</v>
       </c>
       <c r="M199" t="s">
-        <v>25</v>
+        <v>283</v>
       </c>
       <c r="N199" t="s">
-        <v>25</v>
+        <v>150</v>
       </c>
       <c r="O199" t="s">
-        <v>25</v>
+        <v>251</v>
       </c>
       <c r="P199" t="s">
         <v>27</v>
       </c>
       <c r="Q199" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="200" spans="1:21">
@@ -9493,10 +9517,10 @@
         <v>220</v>
       </c>
       <c r="B200" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C200" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="D200" t="s">
         <v>23</v>
@@ -9511,13 +9535,13 @@
         <v>1300</v>
       </c>
       <c r="M200" t="s">
-        <v>25</v>
+        <v>174</v>
       </c>
       <c r="N200" t="s">
-        <v>25</v>
+        <v>230</v>
       </c>
       <c r="O200" t="s">
-        <v>25</v>
+        <v>251</v>
       </c>
       <c r="P200" t="s">
         <v>27</v>
@@ -9531,10 +9555,10 @@
         <v>220</v>
       </c>
       <c r="B201" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C201" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="D201" t="s">
         <v>23</v>
@@ -9542,6 +9566,12 @@
       <c r="E201">
         <v>1450</v>
       </c>
+      <c r="F201">
+        <v>750</v>
+      </c>
+      <c r="G201">
+        <v>750</v>
+      </c>
       <c r="M201" t="s">
         <v>174</v>
       </c>
@@ -9566,7 +9596,7 @@
         <v>221</v>
       </c>
       <c r="C202" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D202" t="s">
         <v>23</v>
@@ -9581,13 +9611,13 @@
         <v>1300</v>
       </c>
       <c r="M202" t="s">
-        <v>25</v>
+        <v>149</v>
       </c>
       <c r="N202" t="s">
-        <v>25</v>
+        <v>287</v>
       </c>
       <c r="O202" t="s">
-        <v>25</v>
+        <v>251</v>
       </c>
       <c r="P202" t="s">
         <v>27</v>
@@ -9604,7 +9634,7 @@
         <v>225</v>
       </c>
       <c r="C203" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D203" t="s">
         <v>23</v>
@@ -9622,7 +9652,7 @@
         <v>149</v>
       </c>
       <c r="N203" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="O203" t="s">
         <v>251</v>
@@ -9639,10 +9669,10 @@
         <v>220</v>
       </c>
       <c r="B204" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C204" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="D204" t="s">
         <v>23</v>
@@ -9657,13 +9687,13 @@
         <v>1300</v>
       </c>
       <c r="M204" t="s">
-        <v>25</v>
+        <v>212</v>
       </c>
       <c r="N204" t="s">
-        <v>25</v>
+        <v>230</v>
       </c>
       <c r="O204" t="s">
-        <v>25</v>
+        <v>251</v>
       </c>
       <c r="P204" t="s">
         <v>27</v>
@@ -9677,10 +9707,10 @@
         <v>220</v>
       </c>
       <c r="B205" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C205" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="D205" t="s">
         <v>23</v>
@@ -9688,6 +9718,12 @@
       <c r="E205">
         <v>1450</v>
       </c>
+      <c r="F205">
+        <v>750</v>
+      </c>
+      <c r="G205">
+        <v>750</v>
+      </c>
       <c r="M205" t="s">
         <v>212</v>
       </c>
@@ -9709,10 +9745,10 @@
         <v>220</v>
       </c>
       <c r="B206" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C206" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="D206" t="s">
         <v>23</v>
@@ -9747,10 +9783,10 @@
         <v>220</v>
       </c>
       <c r="B207" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C207" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="D207" t="s">
         <v>23</v>
@@ -9758,6 +9794,12 @@
       <c r="E207">
         <v>1450</v>
       </c>
+      <c r="F207">
+        <v>750</v>
+      </c>
+      <c r="G207">
+        <v>750</v>
+      </c>
       <c r="M207" t="s">
         <v>212</v>
       </c>
@@ -9782,7 +9824,7 @@
         <v>221</v>
       </c>
       <c r="C208" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="D208" t="s">
         <v>23</v>
@@ -9809,7 +9851,7 @@
         <v>27</v>
       </c>
       <c r="Q208" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
     </row>
     <row r="209" spans="1:21">
@@ -9817,10 +9859,10 @@
         <v>220</v>
       </c>
       <c r="B209" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="C209" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="D209" t="s">
         <v>23</v>
@@ -9835,19 +9877,19 @@
         <v>450</v>
       </c>
       <c r="M209" t="s">
-        <v>25</v>
+        <v>227</v>
       </c>
       <c r="N209" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O209" t="s">
-        <v>25</v>
+        <v>251</v>
       </c>
       <c r="P209" t="s">
         <v>27</v>
       </c>
       <c r="Q209" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
     </row>
     <row r="210" spans="1:21">
@@ -9858,7 +9900,7 @@
         <v>221</v>
       </c>
       <c r="C210" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="D210" t="s">
         <v>23</v>
@@ -9873,10 +9915,10 @@
         <v>1700</v>
       </c>
       <c r="M210" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="N210" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="O210" t="s">
         <v>251</v>
@@ -9896,7 +9938,7 @@
         <v>225</v>
       </c>
       <c r="C211" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="D211" t="s">
         <v>23</v>
@@ -9911,13 +9953,13 @@
         <v>1750</v>
       </c>
       <c r="M211" t="s">
-        <v>25</v>
+        <v>298</v>
       </c>
       <c r="N211" t="s">
-        <v>25</v>
+        <v>299</v>
       </c>
       <c r="O211" t="s">
-        <v>25</v>
+        <v>251</v>
       </c>
       <c r="P211" t="s">
         <v>27</v>
@@ -9934,7 +9976,7 @@
         <v>221</v>
       </c>
       <c r="C212" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="D212" t="s">
         <v>23</v>
@@ -9949,13 +9991,13 @@
         <v>900</v>
       </c>
       <c r="M212" t="s">
-        <v>25</v>
+        <v>301</v>
       </c>
       <c r="N212" t="s">
-        <v>25</v>
+        <v>299</v>
       </c>
       <c r="O212" t="s">
-        <v>25</v>
+        <v>302</v>
       </c>
       <c r="P212" t="s">
         <v>27</v>
@@ -9972,7 +10014,7 @@
         <v>225</v>
       </c>
       <c r="C213" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="D213" t="s">
         <v>23</v>
@@ -9987,13 +10029,13 @@
         <v>950</v>
       </c>
       <c r="M213" t="s">
-        <v>25</v>
+        <v>301</v>
       </c>
       <c r="N213" t="s">
-        <v>25</v>
+        <v>299</v>
       </c>
       <c r="O213" t="s">
-        <v>25</v>
+        <v>302</v>
       </c>
       <c r="P213" t="s">
         <v>27</v>
@@ -10010,7 +10052,7 @@
         <v>221</v>
       </c>
       <c r="C214" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="D214" t="s">
         <v>23</v>
@@ -10025,13 +10067,13 @@
         <v>1700</v>
       </c>
       <c r="M214" t="s">
-        <v>25</v>
+        <v>301</v>
       </c>
       <c r="N214" t="s">
-        <v>25</v>
+        <v>299</v>
       </c>
       <c r="O214" t="s">
-        <v>25</v>
+        <v>302</v>
       </c>
       <c r="P214" t="s">
         <v>27</v>
@@ -10048,7 +10090,7 @@
         <v>225</v>
       </c>
       <c r="C215" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="D215" t="s">
         <v>23</v>
@@ -10063,13 +10105,13 @@
         <v>1750</v>
       </c>
       <c r="M215" t="s">
-        <v>25</v>
+        <v>301</v>
       </c>
       <c r="N215" t="s">
-        <v>25</v>
+        <v>299</v>
       </c>
       <c r="O215" t="s">
-        <v>25</v>
+        <v>302</v>
       </c>
       <c r="P215" t="s">
         <v>27</v>
@@ -10086,7 +10128,7 @@
         <v>221</v>
       </c>
       <c r="C216" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="D216" t="s">
         <v>23</v>
@@ -10101,19 +10143,19 @@
         <v>400</v>
       </c>
       <c r="M216" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="N216" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O216" t="s">
-        <v>25</v>
+        <v>305</v>
       </c>
       <c r="P216" t="s">
         <v>27</v>
       </c>
       <c r="Q216" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
     </row>
     <row r="217" spans="1:21">
@@ -10121,10 +10163,10 @@
         <v>220</v>
       </c>
       <c r="B217" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="C217" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="D217" t="s">
         <v>23</v>
@@ -10139,19 +10181,19 @@
         <v>500</v>
       </c>
       <c r="M217" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="N217" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O217" t="s">
-        <v>25</v>
+        <v>305</v>
       </c>
       <c r="P217" t="s">
         <v>27</v>
       </c>
       <c r="Q217" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
     </row>
     <row r="218" spans="1:21">
@@ -10162,7 +10204,7 @@
         <v>221</v>
       </c>
       <c r="C218" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="D218" t="s">
         <v>23</v>
@@ -10177,19 +10219,19 @@
         <v>600</v>
       </c>
       <c r="M218" t="s">
-        <v>25</v>
+        <v>283</v>
       </c>
       <c r="N218" t="s">
-        <v>25</v>
+        <v>308</v>
       </c>
       <c r="O218" t="s">
-        <v>25</v>
+        <v>305</v>
       </c>
       <c r="P218" t="s">
         <v>27</v>
       </c>
       <c r="Q218" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
     </row>
     <row r="219" spans="1:21">
@@ -10197,10 +10239,10 @@
         <v>220</v>
       </c>
       <c r="B219" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="C219" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="D219" t="s">
         <v>23</v>
@@ -10215,19 +10257,19 @@
         <v>750</v>
       </c>
       <c r="M219" t="s">
-        <v>25</v>
+        <v>283</v>
       </c>
       <c r="N219" t="s">
-        <v>25</v>
+        <v>308</v>
       </c>
       <c r="O219" t="s">
-        <v>25</v>
+        <v>305</v>
       </c>
       <c r="P219" t="s">
         <v>27</v>
       </c>
       <c r="Q219" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
     </row>
     <row r="220" spans="1:21">
@@ -10238,7 +10280,7 @@
         <v>221</v>
       </c>
       <c r="C220" t="s">
-        <v>302</v>
+        <v>309</v>
       </c>
       <c r="D220" t="s">
         <v>23</v>
@@ -10253,13 +10295,13 @@
         <v>900</v>
       </c>
       <c r="M220" t="s">
-        <v>25</v>
+        <v>301</v>
       </c>
       <c r="N220" t="s">
-        <v>25</v>
+        <v>299</v>
       </c>
       <c r="O220" t="s">
-        <v>25</v>
+        <v>305</v>
       </c>
       <c r="P220" t="s">
         <v>27</v>
@@ -10276,7 +10318,7 @@
         <v>225</v>
       </c>
       <c r="C221" t="s">
-        <v>302</v>
+        <v>309</v>
       </c>
       <c r="D221" t="s">
         <v>23</v>
@@ -10291,13 +10333,13 @@
         <v>950</v>
       </c>
       <c r="M221" t="s">
-        <v>25</v>
+        <v>301</v>
       </c>
       <c r="N221" t="s">
-        <v>25</v>
+        <v>299</v>
       </c>
       <c r="O221" t="s">
-        <v>25</v>
+        <v>305</v>
       </c>
       <c r="P221" t="s">
         <v>27</v>
@@ -10314,7 +10356,7 @@
         <v>221</v>
       </c>
       <c r="C222" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="D222" t="s">
         <v>23</v>
@@ -10329,13 +10371,13 @@
         <v>1000</v>
       </c>
       <c r="M222" t="s">
-        <v>25</v>
+        <v>301</v>
       </c>
       <c r="N222" t="s">
-        <v>25</v>
+        <v>299</v>
       </c>
       <c r="O222" t="s">
-        <v>25</v>
+        <v>305</v>
       </c>
       <c r="P222" t="s">
         <v>27</v>
@@ -10352,7 +10394,7 @@
         <v>225</v>
       </c>
       <c r="C223" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="D223" t="s">
         <v>23</v>
@@ -10367,13 +10409,13 @@
         <v>1050</v>
       </c>
       <c r="M223" t="s">
-        <v>25</v>
+        <v>301</v>
       </c>
       <c r="N223" t="s">
-        <v>25</v>
+        <v>299</v>
       </c>
       <c r="O223" t="s">
-        <v>25</v>
+        <v>305</v>
       </c>
       <c r="P223" t="s">
         <v>27</v>
@@ -10390,7 +10432,7 @@
         <v>221</v>
       </c>
       <c r="C224" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="D224" t="s">
         <v>23</v>
@@ -10405,13 +10447,13 @@
         <v>1200</v>
       </c>
       <c r="M224" t="s">
-        <v>25</v>
+        <v>301</v>
       </c>
       <c r="N224" t="s">
-        <v>25</v>
+        <v>299</v>
       </c>
       <c r="O224" t="s">
-        <v>25</v>
+        <v>305</v>
       </c>
       <c r="P224" t="s">
         <v>27</v>
@@ -10428,7 +10470,7 @@
         <v>225</v>
       </c>
       <c r="C225" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="D225" t="s">
         <v>23</v>
@@ -10443,13 +10485,13 @@
         <v>1250</v>
       </c>
       <c r="M225" t="s">
-        <v>25</v>
+        <v>301</v>
       </c>
       <c r="N225" t="s">
-        <v>25</v>
+        <v>299</v>
       </c>
       <c r="O225" t="s">
-        <v>25</v>
+        <v>305</v>
       </c>
       <c r="P225" t="s">
         <v>27</v>
@@ -10466,7 +10508,7 @@
         <v>221</v>
       </c>
       <c r="C226" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
       <c r="D226" t="s">
         <v>23</v>
@@ -10481,13 +10523,13 @@
         <v>900</v>
       </c>
       <c r="M226" t="s">
-        <v>25</v>
+        <v>301</v>
       </c>
       <c r="N226" t="s">
-        <v>25</v>
+        <v>241</v>
       </c>
       <c r="O226" t="s">
-        <v>25</v>
+        <v>305</v>
       </c>
       <c r="P226" t="s">
         <v>27</v>
@@ -10504,7 +10546,7 @@
         <v>225</v>
       </c>
       <c r="C227" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
       <c r="D227" t="s">
         <v>23</v>
@@ -10519,13 +10561,13 @@
         <v>950</v>
       </c>
       <c r="M227" t="s">
-        <v>25</v>
+        <v>301</v>
       </c>
       <c r="N227" t="s">
-        <v>25</v>
+        <v>241</v>
       </c>
       <c r="O227" t="s">
-        <v>25</v>
+        <v>305</v>
       </c>
       <c r="P227" t="s">
         <v>27</v>
@@ -10542,7 +10584,7 @@
         <v>221</v>
       </c>
       <c r="C228" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="D228" t="s">
         <v>23</v>
@@ -10557,13 +10599,13 @@
         <v>2600</v>
       </c>
       <c r="M228" t="s">
-        <v>25</v>
+        <v>199</v>
       </c>
       <c r="N228" t="s">
-        <v>25</v>
+        <v>287</v>
       </c>
       <c r="O228" t="s">
-        <v>25</v>
+        <v>305</v>
       </c>
       <c r="P228" t="s">
         <v>27</v>
@@ -10580,7 +10622,7 @@
         <v>225</v>
       </c>
       <c r="C229" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="D229" t="s">
         <v>23</v>
@@ -10595,13 +10637,13 @@
         <v>2650</v>
       </c>
       <c r="M229" t="s">
-        <v>25</v>
+        <v>199</v>
       </c>
       <c r="N229" t="s">
-        <v>25</v>
+        <v>287</v>
       </c>
       <c r="O229" t="s">
-        <v>25</v>
+        <v>305</v>
       </c>
       <c r="P229" t="s">
         <v>27</v>
@@ -10618,7 +10660,7 @@
         <v>221</v>
       </c>
       <c r="C230" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="D230" t="s">
         <v>23</v>
@@ -10633,13 +10675,13 @@
         <v>1800</v>
       </c>
       <c r="M230" t="s">
-        <v>25</v>
+        <v>315</v>
       </c>
       <c r="N230" t="s">
-        <v>25</v>
+        <v>287</v>
       </c>
       <c r="O230" t="s">
-        <v>25</v>
+        <v>305</v>
       </c>
       <c r="P230" t="s">
         <v>27</v>
@@ -10656,7 +10698,7 @@
         <v>225</v>
       </c>
       <c r="C231" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="D231" t="s">
         <v>23</v>
@@ -10671,13 +10713,13 @@
         <v>1850</v>
       </c>
       <c r="M231" t="s">
-        <v>25</v>
+        <v>315</v>
       </c>
       <c r="N231" t="s">
-        <v>25</v>
+        <v>287</v>
       </c>
       <c r="O231" t="s">
-        <v>25</v>
+        <v>305</v>
       </c>
       <c r="P231" t="s">
         <v>27</v>
@@ -10694,7 +10736,7 @@
         <v>221</v>
       </c>
       <c r="C232" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="D232" t="s">
         <v>23</v>
@@ -10709,19 +10751,19 @@
         <v>350</v>
       </c>
       <c r="M232" t="s">
-        <v>25</v>
+        <v>178</v>
       </c>
       <c r="N232" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O232" t="s">
-        <v>25</v>
+        <v>317</v>
       </c>
       <c r="P232" t="s">
         <v>27</v>
       </c>
       <c r="Q232" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
     </row>
     <row r="233" spans="1:21">
@@ -10732,28 +10774,34 @@
         <v>225</v>
       </c>
       <c r="C233" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="D233" t="s">
         <v>23</v>
       </c>
       <c r="E233">
+        <v>300</v>
+      </c>
+      <c r="F233">
         <v>450</v>
       </c>
+      <c r="G233">
+        <v>450</v>
+      </c>
       <c r="M233" t="s">
-        <v>25</v>
+        <v>178</v>
       </c>
       <c r="N233" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O233" t="s">
-        <v>25</v>
+        <v>317</v>
       </c>
       <c r="P233" t="s">
         <v>27</v>
       </c>
-      <c r="Q233">
-        <v>300</v>
+      <c r="Q233" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="234" spans="1:21">
@@ -10764,7 +10812,7 @@
         <v>221</v>
       </c>
       <c r="C234" t="s">
-        <v>310</v>
+        <v>319</v>
       </c>
       <c r="D234" t="s">
         <v>23</v>
@@ -10779,19 +10827,19 @@
         <v>500</v>
       </c>
       <c r="M234" t="s">
-        <v>25</v>
+        <v>149</v>
       </c>
       <c r="N234" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O234" t="s">
-        <v>25</v>
+        <v>317</v>
       </c>
       <c r="P234" t="s">
         <v>27</v>
       </c>
       <c r="Q234" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="235" spans="1:21">
@@ -10802,28 +10850,34 @@
         <v>225</v>
       </c>
       <c r="C235" t="s">
-        <v>310</v>
+        <v>319</v>
       </c>
       <c r="D235" t="s">
         <v>23</v>
       </c>
       <c r="E235">
+        <v>350</v>
+      </c>
+      <c r="F235">
         <v>600</v>
       </c>
+      <c r="G235">
+        <v>600</v>
+      </c>
       <c r="M235" t="s">
-        <v>25</v>
+        <v>149</v>
       </c>
       <c r="N235" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O235" t="s">
-        <v>25</v>
+        <v>317</v>
       </c>
       <c r="P235" t="s">
         <v>27</v>
       </c>
-      <c r="Q235">
-        <v>350</v>
+      <c r="Q235" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="236" spans="1:21">
@@ -10834,7 +10888,7 @@
         <v>221</v>
       </c>
       <c r="C236" t="s">
-        <v>311</v>
+        <v>320</v>
       </c>
       <c r="D236" t="s">
         <v>23</v>
@@ -10849,13 +10903,13 @@
         <v>450</v>
       </c>
       <c r="M236" t="s">
-        <v>25</v>
+        <v>149</v>
       </c>
       <c r="N236" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O236" t="s">
-        <v>25</v>
+        <v>321</v>
       </c>
       <c r="P236" t="s">
         <v>27</v>
@@ -10872,28 +10926,34 @@
         <v>225</v>
       </c>
       <c r="C237" t="s">
-        <v>311</v>
+        <v>320</v>
       </c>
       <c r="D237" t="s">
         <v>23</v>
       </c>
       <c r="E237">
+        <v>300</v>
+      </c>
+      <c r="F237">
         <v>500</v>
       </c>
+      <c r="G237">
+        <v>500</v>
+      </c>
       <c r="M237" t="s">
-        <v>25</v>
+        <v>149</v>
       </c>
       <c r="N237" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O237" t="s">
-        <v>25</v>
+        <v>321</v>
       </c>
       <c r="P237" t="s">
         <v>27</v>
       </c>
-      <c r="Q237">
-        <v>300</v>
+      <c r="Q237" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="238" spans="1:21">
@@ -10904,7 +10964,7 @@
         <v>221</v>
       </c>
       <c r="C238" t="s">
-        <v>312</v>
+        <v>322</v>
       </c>
       <c r="D238" t="s">
         <v>23</v>
@@ -10919,19 +10979,19 @@
         <v>500</v>
       </c>
       <c r="M238" t="s">
-        <v>25</v>
+        <v>149</v>
       </c>
       <c r="N238" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O238" t="s">
-        <v>25</v>
+        <v>321</v>
       </c>
       <c r="P238" t="s">
         <v>27</v>
       </c>
       <c r="Q238" t="s">
-        <v>313</v>
+        <v>323</v>
       </c>
     </row>
     <row r="239" spans="1:21">
@@ -10942,28 +11002,34 @@
         <v>225</v>
       </c>
       <c r="C239" t="s">
-        <v>312</v>
+        <v>322</v>
       </c>
       <c r="D239" t="s">
         <v>23</v>
       </c>
       <c r="E239">
+        <v>350</v>
+      </c>
+      <c r="F239">
         <v>600</v>
       </c>
+      <c r="G239">
+        <v>600</v>
+      </c>
       <c r="M239" t="s">
-        <v>25</v>
+        <v>149</v>
       </c>
       <c r="N239" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O239" t="s">
-        <v>25</v>
+        <v>321</v>
       </c>
       <c r="P239" t="s">
         <v>27</v>
       </c>
-      <c r="Q239">
-        <v>350</v>
+      <c r="Q239" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="240" spans="1:21">
@@ -10974,7 +11040,7 @@
         <v>221</v>
       </c>
       <c r="C240" t="s">
-        <v>314</v>
+        <v>324</v>
       </c>
       <c r="D240" t="s">
         <v>23</v>
@@ -10989,19 +11055,19 @@
         <v>450</v>
       </c>
       <c r="M240" t="s">
-        <v>25</v>
+        <v>325</v>
       </c>
       <c r="N240" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O240" t="s">
-        <v>25</v>
+        <v>321</v>
       </c>
       <c r="P240" t="s">
         <v>27</v>
       </c>
       <c r="Q240" t="s">
-        <v>315</v>
+        <v>326</v>
       </c>
     </row>
     <row r="241" spans="1:21">
@@ -11012,28 +11078,34 @@
         <v>225</v>
       </c>
       <c r="C241" t="s">
-        <v>314</v>
+        <v>324</v>
       </c>
       <c r="D241" t="s">
         <v>23</v>
       </c>
       <c r="E241">
+        <v>300</v>
+      </c>
+      <c r="F241">
         <v>500</v>
       </c>
+      <c r="G241">
+        <v>500</v>
+      </c>
       <c r="M241" t="s">
-        <v>25</v>
+        <v>325</v>
       </c>
       <c r="N241" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O241" t="s">
-        <v>25</v>
+        <v>321</v>
       </c>
       <c r="P241" t="s">
         <v>27</v>
       </c>
-      <c r="Q241">
-        <v>300</v>
+      <c r="Q241" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="242" spans="1:21">
@@ -11044,7 +11116,7 @@
         <v>221</v>
       </c>
       <c r="C242" t="s">
-        <v>316</v>
+        <v>327</v>
       </c>
       <c r="D242" t="s">
         <v>23</v>
@@ -11059,19 +11131,19 @@
         <v>450</v>
       </c>
       <c r="M242" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="N242" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O242" t="s">
-        <v>25</v>
+        <v>321</v>
       </c>
       <c r="P242" t="s">
         <v>27</v>
       </c>
       <c r="Q242" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="243" spans="1:21">
@@ -11082,28 +11154,34 @@
         <v>225</v>
       </c>
       <c r="C243" t="s">
-        <v>316</v>
+        <v>327</v>
       </c>
       <c r="D243" t="s">
         <v>23</v>
       </c>
       <c r="E243">
+        <v>300</v>
+      </c>
+      <c r="F243">
         <v>500</v>
       </c>
+      <c r="G243">
+        <v>500</v>
+      </c>
       <c r="M243" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="N243" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O243" t="s">
-        <v>25</v>
+        <v>321</v>
       </c>
       <c r="P243" t="s">
         <v>27</v>
       </c>
-      <c r="Q243">
-        <v>300</v>
+      <c r="Q243" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="244" spans="1:21">
@@ -11114,7 +11192,7 @@
         <v>221</v>
       </c>
       <c r="C244" t="s">
-        <v>317</v>
+        <v>328</v>
       </c>
       <c r="D244" t="s">
         <v>23</v>
@@ -11129,19 +11207,19 @@
         <v>450</v>
       </c>
       <c r="M244" t="s">
-        <v>25</v>
+        <v>149</v>
       </c>
       <c r="N244" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O244" t="s">
-        <v>25</v>
+        <v>321</v>
       </c>
       <c r="P244" t="s">
         <v>27</v>
       </c>
       <c r="Q244" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="245" spans="1:21">
@@ -11152,28 +11230,34 @@
         <v>225</v>
       </c>
       <c r="C245" t="s">
-        <v>317</v>
+        <v>328</v>
       </c>
       <c r="D245" t="s">
         <v>23</v>
       </c>
       <c r="E245">
+        <v>300</v>
+      </c>
+      <c r="F245">
         <v>500</v>
       </c>
+      <c r="G245">
+        <v>500</v>
+      </c>
       <c r="M245" t="s">
-        <v>25</v>
+        <v>149</v>
       </c>
       <c r="N245" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O245" t="s">
-        <v>25</v>
+        <v>321</v>
       </c>
       <c r="P245" t="s">
         <v>27</v>
       </c>
-      <c r="Q245">
-        <v>300</v>
+      <c r="Q245" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="246" spans="1:21">
@@ -11184,7 +11268,7 @@
         <v>221</v>
       </c>
       <c r="C246" t="s">
-        <v>318</v>
+        <v>329</v>
       </c>
       <c r="D246" t="s">
         <v>23</v>
@@ -11199,19 +11283,19 @@
         <v>450</v>
       </c>
       <c r="M246" t="s">
-        <v>25</v>
+        <v>330</v>
       </c>
       <c r="N246" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O246" t="s">
-        <v>25</v>
+        <v>331</v>
       </c>
       <c r="P246" t="s">
         <v>27</v>
       </c>
       <c r="Q246" t="s">
-        <v>313</v>
+        <v>323</v>
       </c>
     </row>
     <row r="247" spans="1:21">
@@ -11222,28 +11306,34 @@
         <v>225</v>
       </c>
       <c r="C247" t="s">
-        <v>318</v>
+        <v>329</v>
       </c>
       <c r="D247" t="s">
         <v>23</v>
       </c>
       <c r="E247">
+        <v>300</v>
+      </c>
+      <c r="F247">
         <v>500</v>
       </c>
+      <c r="G247">
+        <v>500</v>
+      </c>
       <c r="M247" t="s">
-        <v>25</v>
+        <v>330</v>
       </c>
       <c r="N247" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O247" t="s">
-        <v>25</v>
+        <v>331</v>
       </c>
       <c r="P247" t="s">
         <v>27</v>
       </c>
-      <c r="Q247">
-        <v>300</v>
+      <c r="Q247" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="248" spans="1:21">
@@ -11254,7 +11344,7 @@
         <v>221</v>
       </c>
       <c r="C248" t="s">
-        <v>319</v>
+        <v>332</v>
       </c>
       <c r="D248" t="s">
         <v>23</v>
@@ -11292,14 +11382,20 @@
         <v>225</v>
       </c>
       <c r="C249" t="s">
-        <v>319</v>
+        <v>332</v>
       </c>
       <c r="D249" t="s">
         <v>23</v>
       </c>
       <c r="E249">
+        <v>380</v>
+      </c>
+      <c r="F249">
         <v>600</v>
       </c>
+      <c r="G249">
+        <v>600</v>
+      </c>
       <c r="M249" t="s">
         <v>25</v>
       </c>
@@ -11312,8 +11408,8 @@
       <c r="P249" t="s">
         <v>27</v>
       </c>
-      <c r="Q249">
-        <v>380</v>
+      <c r="Q249" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="250" spans="1:21">
@@ -11321,10 +11417,10 @@
         <v>220</v>
       </c>
       <c r="B250" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C250" t="s">
-        <v>320</v>
+        <v>333</v>
       </c>
       <c r="D250" t="s">
         <v>23</v>
@@ -11359,10 +11455,10 @@
         <v>220</v>
       </c>
       <c r="B251" t="s">
-        <v>321</v>
+        <v>334</v>
       </c>
       <c r="C251" t="s">
-        <v>320</v>
+        <v>333</v>
       </c>
       <c r="D251" t="s">
         <v>23</v>
@@ -11397,10 +11493,10 @@
         <v>220</v>
       </c>
       <c r="B252" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C252" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="D252" t="s">
         <v>23</v>
@@ -11435,10 +11531,10 @@
         <v>220</v>
       </c>
       <c r="B253" t="s">
-        <v>321</v>
+        <v>334</v>
       </c>
       <c r="C253" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="D253" t="s">
         <v>23</v>
@@ -11473,10 +11569,10 @@
         <v>220</v>
       </c>
       <c r="B254" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C254" t="s">
-        <v>323</v>
+        <v>336</v>
       </c>
       <c r="D254" t="s">
         <v>23</v>
@@ -11511,10 +11607,10 @@
         <v>220</v>
       </c>
       <c r="B255" t="s">
-        <v>321</v>
+        <v>334</v>
       </c>
       <c r="C255" t="s">
-        <v>323</v>
+        <v>336</v>
       </c>
       <c r="D255" t="s">
         <v>23</v>
@@ -11549,10 +11645,10 @@
         <v>220</v>
       </c>
       <c r="B256" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C256" t="s">
-        <v>324</v>
+        <v>337</v>
       </c>
       <c r="D256" t="s">
         <v>23</v>
@@ -11587,10 +11683,10 @@
         <v>220</v>
       </c>
       <c r="B257" t="s">
-        <v>321</v>
+        <v>334</v>
       </c>
       <c r="C257" t="s">
-        <v>324</v>
+        <v>337</v>
       </c>
       <c r="D257" t="s">
         <v>23</v>
@@ -11625,10 +11721,10 @@
         <v>220</v>
       </c>
       <c r="B258" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C258" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="D258" t="s">
         <v>23</v>
@@ -11663,10 +11759,10 @@
         <v>220</v>
       </c>
       <c r="B259" t="s">
-        <v>321</v>
+        <v>334</v>
       </c>
       <c r="C259" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="D259" t="s">
         <v>23</v>
@@ -11701,10 +11797,10 @@
         <v>220</v>
       </c>
       <c r="B260" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C260" t="s">
-        <v>326</v>
+        <v>339</v>
       </c>
       <c r="D260" t="s">
         <v>23</v>
@@ -11739,10 +11835,10 @@
         <v>220</v>
       </c>
       <c r="B261" t="s">
-        <v>321</v>
+        <v>334</v>
       </c>
       <c r="C261" t="s">
-        <v>326</v>
+        <v>339</v>
       </c>
       <c r="D261" t="s">
         <v>23</v>
@@ -11777,10 +11873,10 @@
         <v>220</v>
       </c>
       <c r="B262" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C262" t="s">
-        <v>327</v>
+        <v>340</v>
       </c>
       <c r="D262" t="s">
         <v>23</v>
@@ -11815,10 +11911,10 @@
         <v>220</v>
       </c>
       <c r="B263" t="s">
-        <v>321</v>
+        <v>334</v>
       </c>
       <c r="C263" t="s">
-        <v>327</v>
+        <v>340</v>
       </c>
       <c r="D263" t="s">
         <v>23</v>
@@ -11853,10 +11949,10 @@
         <v>220</v>
       </c>
       <c r="B264" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C264" t="s">
-        <v>328</v>
+        <v>341</v>
       </c>
       <c r="D264" t="s">
         <v>23</v>
@@ -11891,10 +11987,10 @@
         <v>220</v>
       </c>
       <c r="B265" t="s">
-        <v>321</v>
+        <v>334</v>
       </c>
       <c r="C265" t="s">
-        <v>328</v>
+        <v>341</v>
       </c>
       <c r="D265" t="s">
         <v>23</v>
@@ -11929,10 +12025,10 @@
         <v>220</v>
       </c>
       <c r="B266" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C266" t="s">
-        <v>329</v>
+        <v>342</v>
       </c>
       <c r="D266" t="s">
         <v>23</v>
@@ -11967,10 +12063,10 @@
         <v>220</v>
       </c>
       <c r="B267" t="s">
-        <v>321</v>
+        <v>334</v>
       </c>
       <c r="C267" t="s">
-        <v>329</v>
+        <v>342</v>
       </c>
       <c r="D267" t="s">
         <v>23</v>
@@ -12005,10 +12101,10 @@
         <v>220</v>
       </c>
       <c r="B268" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C268" t="s">
-        <v>330</v>
+        <v>343</v>
       </c>
       <c r="D268" t="s">
         <v>23</v>
@@ -12043,10 +12139,10 @@
         <v>220</v>
       </c>
       <c r="B269" t="s">
-        <v>321</v>
+        <v>334</v>
       </c>
       <c r="C269" t="s">
-        <v>330</v>
+        <v>343</v>
       </c>
       <c r="D269" t="s">
         <v>23</v>
@@ -12081,10 +12177,10 @@
         <v>220</v>
       </c>
       <c r="B270" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C270" t="s">
-        <v>331</v>
+        <v>344</v>
       </c>
       <c r="D270" t="s">
         <v>23</v>
@@ -12111,7 +12207,7 @@
         <v>27</v>
       </c>
       <c r="Q270" t="s">
-        <v>332</v>
+        <v>345</v>
       </c>
     </row>
     <row r="271" spans="1:21">
@@ -12119,10 +12215,10 @@
         <v>220</v>
       </c>
       <c r="B271" t="s">
-        <v>321</v>
+        <v>334</v>
       </c>
       <c r="C271" t="s">
-        <v>331</v>
+        <v>344</v>
       </c>
       <c r="D271" t="s">
         <v>23</v>
@@ -12149,7 +12245,7 @@
         <v>27</v>
       </c>
       <c r="Q271" t="s">
-        <v>332</v>
+        <v>345</v>
       </c>
     </row>
     <row r="272" spans="1:21">
@@ -12157,10 +12253,10 @@
         <v>220</v>
       </c>
       <c r="B272" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C272" t="s">
-        <v>333</v>
+        <v>346</v>
       </c>
       <c r="D272" t="s">
         <v>23</v>
@@ -12187,7 +12283,7 @@
         <v>27</v>
       </c>
       <c r="Q272" t="s">
-        <v>332</v>
+        <v>345</v>
       </c>
     </row>
     <row r="273" spans="1:21">
@@ -12195,10 +12291,10 @@
         <v>220</v>
       </c>
       <c r="B273" t="s">
-        <v>321</v>
+        <v>334</v>
       </c>
       <c r="C273" t="s">
-        <v>333</v>
+        <v>346</v>
       </c>
       <c r="D273" t="s">
         <v>23</v>
@@ -12225,7 +12321,7 @@
         <v>27</v>
       </c>
       <c r="Q273" t="s">
-        <v>332</v>
+        <v>345</v>
       </c>
     </row>
     <row r="274" spans="1:21">
@@ -12233,10 +12329,10 @@
         <v>220</v>
       </c>
       <c r="B274" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C274" t="s">
-        <v>334</v>
+        <v>347</v>
       </c>
       <c r="D274" t="s">
         <v>23</v>
@@ -12271,10 +12367,10 @@
         <v>220</v>
       </c>
       <c r="B275" t="s">
-        <v>321</v>
+        <v>334</v>
       </c>
       <c r="C275" t="s">
-        <v>334</v>
+        <v>347</v>
       </c>
       <c r="D275" t="s">
         <v>23</v>
@@ -12312,7 +12408,7 @@
         <v>221</v>
       </c>
       <c r="C276" t="s">
-        <v>335</v>
+        <v>348</v>
       </c>
       <c r="D276" t="s">
         <v>23</v>
@@ -12350,14 +12446,20 @@
         <v>225</v>
       </c>
       <c r="C277" t="s">
-        <v>335</v>
+        <v>348</v>
       </c>
       <c r="D277" t="s">
         <v>23</v>
       </c>
       <c r="E277">
+        <v>1150</v>
+      </c>
+      <c r="F277">
         <v>1400</v>
       </c>
+      <c r="G277">
+        <v>1400</v>
+      </c>
       <c r="M277" t="s">
         <v>25</v>
       </c>
@@ -12371,7 +12473,7 @@
         <v>27</v>
       </c>
       <c r="Q277" t="s">
-        <v>336</v>
+        <v>239</v>
       </c>
     </row>
     <row r="278" spans="1:21">
@@ -12382,7 +12484,7 @@
         <v>221</v>
       </c>
       <c r="C278" t="s">
-        <v>337</v>
+        <v>349</v>
       </c>
       <c r="D278" t="s">
         <v>23</v>
@@ -12420,14 +12522,20 @@
         <v>225</v>
       </c>
       <c r="C279" t="s">
-        <v>337</v>
+        <v>349</v>
       </c>
       <c r="D279" t="s">
         <v>23</v>
       </c>
       <c r="E279">
+        <v>1550</v>
+      </c>
+      <c r="F279">
         <v>2250</v>
       </c>
+      <c r="G279">
+        <v>2250</v>
+      </c>
       <c r="M279" t="s">
         <v>25</v>
       </c>
@@ -12441,7 +12549,7 @@
         <v>27</v>
       </c>
       <c r="Q279" t="s">
-        <v>338</v>
+        <v>239</v>
       </c>
     </row>
     <row r="280" spans="1:21">
@@ -12452,7 +12560,7 @@
         <v>221</v>
       </c>
       <c r="C280" t="s">
-        <v>339</v>
+        <v>350</v>
       </c>
       <c r="D280" t="s">
         <v>23</v>
@@ -12490,14 +12598,20 @@
         <v>225</v>
       </c>
       <c r="C281" t="s">
-        <v>339</v>
+        <v>350</v>
       </c>
       <c r="D281" t="s">
         <v>23</v>
       </c>
       <c r="E281">
+        <v>1530</v>
+      </c>
+      <c r="F281">
         <v>2100</v>
       </c>
+      <c r="G281">
+        <v>2100</v>
+      </c>
       <c r="M281" t="s">
         <v>25</v>
       </c>
@@ -12511,7 +12625,7 @@
         <v>27</v>
       </c>
       <c r="Q281" t="s">
-        <v>340</v>
+        <v>239</v>
       </c>
     </row>
     <row r="282" spans="1:21">
@@ -12522,7 +12636,7 @@
         <v>221</v>
       </c>
       <c r="C282" t="s">
-        <v>341</v>
+        <v>351</v>
       </c>
       <c r="D282" t="s">
         <v>23</v>
@@ -12557,17 +12671,23 @@
         <v>220</v>
       </c>
       <c r="B283" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C283" t="s">
-        <v>341</v>
+        <v>351</v>
       </c>
       <c r="D283" t="s">
         <v>23</v>
       </c>
       <c r="E283">
+        <v>1250</v>
+      </c>
+      <c r="F283">
         <v>1600</v>
       </c>
+      <c r="G283">
+        <v>1600</v>
+      </c>
       <c r="M283" t="s">
         <v>25</v>
       </c>
@@ -12581,7 +12701,7 @@
         <v>27</v>
       </c>
       <c r="Q283" t="s">
-        <v>343</v>
+        <v>239</v>
       </c>
     </row>
     <row r="284" spans="1:21">
@@ -12592,7 +12712,7 @@
         <v>221</v>
       </c>
       <c r="C284" t="s">
-        <v>344</v>
+        <v>353</v>
       </c>
       <c r="D284" t="s">
         <v>23</v>
@@ -12627,17 +12747,23 @@
         <v>220</v>
       </c>
       <c r="B285" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C285" t="s">
-        <v>344</v>
+        <v>353</v>
       </c>
       <c r="D285" t="s">
         <v>23</v>
       </c>
       <c r="E285">
+        <v>1250</v>
+      </c>
+      <c r="F285">
         <v>1600</v>
       </c>
+      <c r="G285">
+        <v>1600</v>
+      </c>
       <c r="M285" t="s">
         <v>25</v>
       </c>
@@ -12651,7 +12777,7 @@
         <v>27</v>
       </c>
       <c r="Q285" t="s">
-        <v>343</v>
+        <v>239</v>
       </c>
     </row>
     <row r="286" spans="1:21">
@@ -12659,22 +12785,22 @@
         <v>220</v>
       </c>
       <c r="B286" t="s">
-        <v>345</v>
+        <v>354</v>
       </c>
       <c r="C286" t="s">
-        <v>346</v>
+        <v>355</v>
       </c>
       <c r="D286" t="s">
         <v>23</v>
       </c>
-      <c r="E286" t="s">
+      <c r="E286">
+        <v>10</v>
+      </c>
+      <c r="F286" t="s">
         <v>26</v>
       </c>
-      <c r="F286" t="s">
-        <v>347</v>
-      </c>
       <c r="G286" t="s">
-        <v>347</v>
+        <v>26</v>
       </c>
       <c r="M286" t="s">
         <v>25</v>
@@ -12688,8 +12814,8 @@
       <c r="P286" t="s">
         <v>27</v>
       </c>
-      <c r="Q286">
-        <v>10</v>
+      <c r="Q286" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="287" spans="1:21">
@@ -12697,22 +12823,22 @@
         <v>220</v>
       </c>
       <c r="B287" t="s">
-        <v>348</v>
+        <v>356</v>
       </c>
       <c r="C287" t="s">
-        <v>346</v>
+        <v>355</v>
       </c>
       <c r="D287" t="s">
         <v>23</v>
       </c>
       <c r="E287" t="s">
-        <v>349</v>
+        <v>357</v>
       </c>
       <c r="F287" t="s">
-        <v>347</v>
+        <v>321</v>
       </c>
       <c r="G287" t="s">
-        <v>347</v>
+        <v>321</v>
       </c>
       <c r="M287" t="s">
         <v>25</v>
@@ -12727,7 +12853,7 @@
         <v>27</v>
       </c>
       <c r="Q287" t="s">
-        <v>350</v>
+        <v>358</v>
       </c>
     </row>
     <row r="288" spans="1:21">
@@ -12735,22 +12861,22 @@
         <v>220</v>
       </c>
       <c r="B288" t="s">
-        <v>345</v>
+        <v>354</v>
       </c>
       <c r="C288" t="s">
-        <v>346</v>
+        <v>355</v>
       </c>
       <c r="D288" t="s">
         <v>23</v>
       </c>
       <c r="E288" t="s">
-        <v>349</v>
+        <v>357</v>
       </c>
       <c r="F288" t="s">
-        <v>347</v>
+        <v>321</v>
       </c>
       <c r="G288" t="s">
-        <v>347</v>
+        <v>321</v>
       </c>
       <c r="M288" t="s">
         <v>25</v>
@@ -12765,7 +12891,7 @@
         <v>27</v>
       </c>
       <c r="Q288" t="s">
-        <v>350</v>
+        <v>358</v>
       </c>
     </row>
     <row r="289" spans="1:21">
@@ -12773,22 +12899,22 @@
         <v>220</v>
       </c>
       <c r="B289" t="s">
-        <v>345</v>
+        <v>354</v>
       </c>
       <c r="C289" t="s">
-        <v>346</v>
+        <v>355</v>
       </c>
       <c r="D289" t="s">
         <v>23</v>
       </c>
       <c r="E289" t="s">
-        <v>349</v>
+        <v>357</v>
       </c>
       <c r="F289" t="s">
-        <v>351</v>
+        <v>359</v>
       </c>
       <c r="G289" t="s">
-        <v>351</v>
+        <v>359</v>
       </c>
       <c r="M289" t="s">
         <v>25</v>
@@ -12803,7 +12929,7 @@
         <v>27</v>
       </c>
       <c r="Q289" t="s">
-        <v>350</v>
+        <v>358</v>
       </c>
     </row>
     <row r="290" spans="1:21">
@@ -12811,10 +12937,10 @@
         <v>220</v>
       </c>
       <c r="B290" t="s">
-        <v>352</v>
+        <v>360</v>
       </c>
       <c r="C290" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="D290" t="s">
         <v>23</v>
@@ -12823,10 +12949,10 @@
         <v>20</v>
       </c>
       <c r="F290" t="s">
-        <v>353</v>
+        <v>361</v>
       </c>
       <c r="G290" t="s">
-        <v>353</v>
+        <v>361</v>
       </c>
       <c r="M290" t="s">
         <v>25</v>
@@ -12846,16 +12972,16 @@
         <v>220</v>
       </c>
       <c r="B291" t="s">
-        <v>354</v>
+        <v>362</v>
       </c>
       <c r="C291" t="s">
-        <v>355</v>
+        <v>363</v>
       </c>
       <c r="D291" t="s">
         <v>23</v>
       </c>
       <c r="E291" t="s">
-        <v>356</v>
+        <v>364</v>
       </c>
       <c r="M291" t="s">
         <v>25</v>
@@ -12870,7 +12996,7 @@
         <v>27</v>
       </c>
       <c r="Q291" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="292" spans="1:21">
@@ -12878,10 +13004,10 @@
         <v>220</v>
       </c>
       <c r="B292" t="s">
-        <v>354</v>
+        <v>362</v>
       </c>
       <c r="C292" t="s">
-        <v>355</v>
+        <v>363</v>
       </c>
       <c r="D292" t="s">
         <v>23</v>
@@ -12890,10 +13016,10 @@
         <v>33</v>
       </c>
       <c r="F292" t="s">
-        <v>357</v>
+        <v>365</v>
       </c>
       <c r="G292" t="s">
-        <v>357</v>
+        <v>365</v>
       </c>
       <c r="M292" t="s">
         <v>25</v>
@@ -12908,7 +13034,7 @@
         <v>27</v>
       </c>
       <c r="Q292" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="293" spans="1:21">
@@ -12916,10 +13042,10 @@
         <v>220</v>
       </c>
       <c r="B293" t="s">
-        <v>358</v>
+        <v>366</v>
       </c>
       <c r="C293" t="s">
-        <v>357</v>
+        <v>365</v>
       </c>
       <c r="D293" t="s">
         <v>23</v>
@@ -12928,10 +13054,10 @@
         <v>20</v>
       </c>
       <c r="F293" t="s">
-        <v>359</v>
+        <v>367</v>
       </c>
       <c r="G293" t="s">
-        <v>359</v>
+        <v>367</v>
       </c>
       <c r="M293" t="s">
         <v>25</v>
@@ -12951,22 +13077,22 @@
         <v>220</v>
       </c>
       <c r="B294" t="s">
-        <v>360</v>
+        <v>368</v>
       </c>
       <c r="C294" t="s">
-        <v>361</v>
+        <v>369</v>
       </c>
       <c r="D294" t="s">
         <v>23</v>
       </c>
       <c r="E294" t="s">
-        <v>359</v>
+        <v>367</v>
       </c>
       <c r="F294" t="s">
-        <v>356</v>
+        <v>364</v>
       </c>
       <c r="G294" t="s">
-        <v>356</v>
+        <v>364</v>
       </c>
       <c r="M294" t="s">
         <v>25</v>
@@ -12981,7 +13107,7 @@
         <v>27</v>
       </c>
       <c r="Q294" t="s">
-        <v>362</v>
+        <v>370</v>
       </c>
     </row>
     <row r="295" spans="1:21">
@@ -12992,7 +13118,7 @@
         <v>221</v>
       </c>
       <c r="C295" t="s">
-        <v>363</v>
+        <v>371</v>
       </c>
       <c r="D295" t="s">
         <v>23</v>
@@ -13027,17 +13153,23 @@
         <v>220</v>
       </c>
       <c r="B296" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C296" t="s">
-        <v>363</v>
+        <v>371</v>
       </c>
       <c r="D296" t="s">
         <v>23</v>
       </c>
       <c r="E296">
+        <v>1650</v>
+      </c>
+      <c r="F296">
         <v>2300</v>
       </c>
+      <c r="G296">
+        <v>2300</v>
+      </c>
       <c r="M296" t="s">
         <v>25</v>
       </c>
@@ -13051,7 +13183,7 @@
         <v>27</v>
       </c>
       <c r="Q296" t="s">
-        <v>364</v>
+        <v>239</v>
       </c>
     </row>
     <row r="297" spans="1:21">
@@ -13062,7 +13194,7 @@
         <v>221</v>
       </c>
       <c r="C297" t="s">
-        <v>365</v>
+        <v>372</v>
       </c>
       <c r="D297" t="s">
         <v>23</v>
@@ -13097,17 +13229,23 @@
         <v>220</v>
       </c>
       <c r="B298" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C298" t="s">
-        <v>365</v>
+        <v>372</v>
       </c>
       <c r="D298" t="s">
         <v>23</v>
       </c>
       <c r="E298">
+        <v>1850</v>
+      </c>
+      <c r="F298">
         <v>2500</v>
       </c>
+      <c r="G298">
+        <v>2500</v>
+      </c>
       <c r="M298" t="s">
         <v>25</v>
       </c>
@@ -13121,7 +13259,7 @@
         <v>27</v>
       </c>
       <c r="Q298" t="s">
-        <v>366</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>